<commit_message>
almost done only remains 'Coupling feature properties values to Observation'
</commit_message>
<xml_diff>
--- a/Vocabulary/BoreholeIE_consolidated_vocab.xlsx
+++ b/Vocabulary/BoreholeIE_consolidated_vocab.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="486">
   <si>
     <t>Concept</t>
   </si>
@@ -1132,6 +1132,390 @@
   </si>
   <si>
     <t>todo</t>
+  </si>
+  <si>
+    <t>A core run is defined by the drilling that happens during the time in which one core barrel is in the borehole. It starts when drilling succeeds with the empty core barrel and ends when the core barrel is full or has to be retrieved from the borehole for other reasons. The entire drill core retrieved from a borehole is the sum of drill core from all core runs in this borehole. It is also called the sampling material.
+IODP/ICDP naming example: 5054-1-A-178Z (Expedition number-Drill site number-Borehole character-Core run number and coring type designation)</t>
+  </si>
+  <si>
+    <t>Number of the expedition to which this core run belongs to (see concept/feature Expedition).</t>
+  </si>
+  <si>
+    <t>Number of the site to which this core run belongs to (see concept/feature Site).</t>
+  </si>
+  <si>
+    <t>Hole</t>
+  </si>
+  <si>
+    <t>Character code of the borehole from which this core run was retrieved (see concept/feature Borehole).</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Core run number (within borehole; 1,2,...). IODP/ICDP convention.</t>
+  </si>
+  <si>
+    <t>Core type</t>
+  </si>
+  <si>
+    <t>1 character code for the core type according to IODP/ICDP convention (stands for e.g. piston, gravity, diamond core).</t>
+  </si>
+  <si>
+    <t>Top depth</t>
+  </si>
+  <si>
+    <t>Driller's depth at the top of the core (i.e. when drilling of the core run commences).</t>
+  </si>
+  <si>
+    <t>Bottom depth</t>
+  </si>
+  <si>
+    <t>Driller's depth at the bottom of the core (i.e. when the core barrel is pulled out of the hole).</t>
+  </si>
+  <si>
+    <t>Drilled length</t>
+  </si>
+  <si>
+    <t>Drilled length (calculated from top and bottom depths).</t>
+  </si>
+  <si>
+    <t>MCD offset</t>
+  </si>
+  <si>
+    <t>Offset between driller's depth and MCD (mean corrected depth, which is the depth after corrections by the scientists (e.g. after logging)).</t>
+  </si>
+  <si>
+    <t>MCD top</t>
+  </si>
+  <si>
+    <t>Corrected top depth (calculated as Top depth + MCD offset).</t>
+  </si>
+  <si>
+    <t>MCD bottom</t>
+  </si>
+  <si>
+    <t>Corrected bottom depth (calculated as Bottom depth + MCD offset).</t>
+  </si>
+  <si>
+    <t>Core recovery</t>
+  </si>
+  <si>
+    <t>Length of the recovered core as measured by the scientists.</t>
+  </si>
+  <si>
+    <t>Core recovery PC</t>
+  </si>
+  <si>
+    <t>Core recovery in percentage (calculated as Core recovery / Drilled length).</t>
+  </si>
+  <si>
+    <t>Core on deck</t>
+  </si>
+  <si>
+    <t>Time and date when the core arrived on the drill deck.</t>
+  </si>
+  <si>
+    <t>Oriented</t>
+  </si>
+  <si>
+    <t>Boolean value to indicate whether the core run is oriented, i.e. orientation measured by a dedicated device. The values are stored in a different table (need to be included).</t>
+  </si>
+  <si>
+    <t>Last section</t>
+  </si>
+  <si>
+    <t>Number of last section of the core, i.e number of sections in which the core run was subdivided (see definition of section below).</t>
+  </si>
+  <si>
+    <t>Core catcher</t>
+  </si>
+  <si>
+    <t>Boolean value that indicates whether a core catcher section exists or not. Mainly important for unconsolidated sediment cores, where the core catcher might contain additional material.</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Initials of the data operator.</t>
+  </si>
+  <si>
+    <t>Remarks on the core run.</t>
+  </si>
+  <si>
+    <t>IGSN</t>
+  </si>
+  <si>
+    <t>The International GeoSample Number of the core run.</t>
+  </si>
+  <si>
+    <t>Number of the expedition to which this core section belongs to (see concept/feature Expedition).</t>
+  </si>
+  <si>
+    <t>Number of the site to which this core section belongs to (see concept/feature Site).</t>
+  </si>
+  <si>
+    <t>Character code of the borehole from which this core section was retrieved (see concept/feature Borehole).</t>
+  </si>
+  <si>
+    <t>Core run number to which this core section belongs to (see concept/feature Core run).</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Section number within the core run.</t>
+  </si>
+  <si>
+    <t>Init length</t>
+  </si>
+  <si>
+    <t>Length of the core section as measured by the scientist.</t>
+  </si>
+  <si>
+    <t>Curated length</t>
+  </si>
+  <si>
+    <t>The length of the curated core section.</t>
+  </si>
+  <si>
+    <t>Driller's depth at the top of the core section (calculated from values of the core run and the other sections in this core run).</t>
+  </si>
+  <si>
+    <t>Driller's depth at the bottom of the core section (calculated from Top depth and Init length).</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Boolean value that indicates whether this section is the core catcher section or not.</t>
+  </si>
+  <si>
+    <t>Corrected top depth (calculated as Top depth + MCD offset of the core run).</t>
+  </si>
+  <si>
+    <t>Corrected bottom depth (calculated as Bottom depth + MCD offset of the core run).</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>Number of the core box in which this core section is stored (see concept/feature Core box).</t>
+  </si>
+  <si>
+    <t>Slot</t>
+  </si>
+  <si>
+    <t>Number of the core box slot in which this core section is stored (see concept/feature Core box).</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Position of the section in the core box slot (several core sections can be stored in one slot; top, middle, bottom, full).</t>
+  </si>
+  <si>
+    <t>Remarks on the core section.</t>
+  </si>
+  <si>
+    <t>The International GeoSample Number of the core section.</t>
+  </si>
+  <si>
+    <t>A core run consists of one to many core sections. This subdivision is defined by the scientists who handle the core and the ways to do this may vary from project to project.
+IODP/ICDP naming example: 5054-1-A-178Z-3WR (Expedition number-Drill site number-Borehole character-Core run number and coring type designation-Section number and character code for part of section)</t>
+  </si>
+  <si>
+    <t>Part of a core section with common descriptive attributes, used e.g. for visual core description.
+IODP/ICDP naming example: 5054-1-A-178Z-3WR-54 (Expedition number-Drill site number-Borehole character-Core run number and coring type designation-Section number and character code for part of section-cm from top of the section)</t>
+  </si>
+  <si>
+    <t>Number of the expedition to which this core unit belongs to (see concept/feature Expedition).</t>
+  </si>
+  <si>
+    <t>Number of the site to which this core unit belongs to (see concept/feature Site).</t>
+  </si>
+  <si>
+    <t>Character code of the borehole to which this core unit belongs to (see concept/feature Borehole).</t>
+  </si>
+  <si>
+    <t>Core run number to which this core unit belongs to (see concept/feature Core run).</t>
+  </si>
+  <si>
+    <t>Number of the section of which this unit is part of (see concept/feature Core section).</t>
+  </si>
+  <si>
+    <t>Section unit</t>
+  </si>
+  <si>
+    <t>Number of this section unit on the core section.</t>
+  </si>
+  <si>
+    <t>Top interval</t>
+  </si>
+  <si>
+    <t>Distance from the top of the section to the top of the section unit.</t>
+  </si>
+  <si>
+    <t>Driller's depth at the top of the section unit (calculated and stored in the database).</t>
+  </si>
+  <si>
+    <t>Top depth MCD</t>
+  </si>
+  <si>
+    <t>Corrected depth at the top of the section unit (calculated and stored in the database). Should be "MCD Top" in accordance with the naming on core run and core section</t>
+  </si>
+  <si>
+    <t>Various fields to describe the section unit</t>
+  </si>
+  <si>
+    <t>not harmonised (based on requirements from the expedition</t>
+  </si>
+  <si>
+    <t>A core sample is a piece of drill core that is taken from the sampling material in order to perform detailed studies. Afterwards, a sample may be returned to the sampling material or lost (destructive investigations). Hierarchically, the core sample is a part of a core section.</t>
+  </si>
+  <si>
+    <t>Number of the expedition to which this core sample belongs to (see concept/feature Expedition).</t>
+  </si>
+  <si>
+    <t>Number of the site to which this core sample belongs to (see concept/feature Site).</t>
+  </si>
+  <si>
+    <t>Character code of the borehole to which this core sample belongs to (see concept/feature Borehole).</t>
+  </si>
+  <si>
+    <t>Core run number to which the sampled core section belongs to (see concept/feature Core run).</t>
+  </si>
+  <si>
+    <t>Section number of the sampled section (see concept/feature Core section).</t>
+  </si>
+  <si>
+    <t>Half</t>
+  </si>
+  <si>
+    <t>Indicates which part of section is sampled (archive or working half, whole round; IODP/ICDP convention).</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Sample code (if present, the type codes are defined by the expedition, i.e. are unregulated).</t>
+  </si>
+  <si>
+    <t>Relative top depth of the sample (on the section).</t>
+  </si>
+  <si>
+    <t>Relative bottom depth of the sample (on the section)</t>
+  </si>
+  <si>
+    <t>Corrected depth for the top of the sample (calculated as Top depth + MCD offset of the core run).</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Volume of the sample.</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Location identifier, which is a shortcut for the core repository (according to IODP/ICDP convention).</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>Identifier of the sample request for this sample.</t>
+  </si>
+  <si>
+    <t>Request part</t>
+  </si>
+  <si>
+    <t>Identifier of the part of the sample request.</t>
+  </si>
+  <si>
+    <t>Sample date</t>
+  </si>
+  <si>
+    <t>Date and time when the sample was taken.</t>
+  </si>
+  <si>
+    <t>Remarks on the sample/sampling procedure.</t>
+  </si>
+  <si>
+    <t>The International GeoSample Number of the sample.</t>
+  </si>
+  <si>
+    <t>A box with subdivisions for storing core sections. This concept describes the layout and content of a core box, which in reverse describes the location of each core section.</t>
+  </si>
+  <si>
+    <t>Number of the expedition (see concept/feature Expedition).</t>
+  </si>
+  <si>
+    <t>Number of the site to which this core box belongs to (see concept/feature Site).</t>
+  </si>
+  <si>
+    <t>Character code of the borehole from which the drill core in this box was retrieved (see concept/feature Borehole).</t>
+  </si>
+  <si>
+    <t>Number of the core box.</t>
+  </si>
+  <si>
+    <t>Top slot</t>
+  </si>
+  <si>
+    <t>Number of the first slot of the box.</t>
+  </si>
+  <si>
+    <t>Bottom slot</t>
+  </si>
+  <si>
+    <t>Number of the last slot of the box.</t>
+  </si>
+  <si>
+    <t>Driller's depth for the top of the top section in the core box. It is assumed that the boxes are filled consecutively, though not necessarily with continuous core (gaps occur, either due to core loss or uncored drilling intervals).</t>
+  </si>
+  <si>
+    <t>Driller's depth of the bottom of the bottom core section of the core box.</t>
+  </si>
+  <si>
+    <t>Corrected depth for the top of the top section in the core box (calculated as Top depth + MCD offset of the respective core run).</t>
+  </si>
+  <si>
+    <t>MCD Bottom</t>
+  </si>
+  <si>
+    <t>Corrected depth for the bottom of the bottom core section of the core box (calculated as Bottom depth + MCD offset of the respective core run).</t>
+  </si>
+  <si>
+    <t>Top core</t>
+  </si>
+  <si>
+    <t>Core run number for the top section of the core box.</t>
+  </si>
+  <si>
+    <t>Top section</t>
+  </si>
+  <si>
+    <t>Section number for the top section of the core box.</t>
+  </si>
+  <si>
+    <t>Bottom core</t>
+  </si>
+  <si>
+    <t>Core run number for the bottom section of the core box.</t>
+  </si>
+  <si>
+    <t>Bottom section</t>
+  </si>
+  <si>
+    <t>Section number for the bottom section of the core box.</t>
+  </si>
+  <si>
+    <t>Archiving date</t>
+  </si>
+  <si>
+    <t>Archiving date of the core box.</t>
   </si>
 </sst>
 </file>
@@ -1257,7 +1641,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1289,6 +1673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1301,7 +1686,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1310,16 +1698,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1604,8 +1991,8 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M41" sqref="M41"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1820,7 +2207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>54</v>
       </c>
@@ -2163,7 +2550,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="13" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="1"/>
@@ -2184,7 +2571,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B26" s="1"/>
@@ -2205,7 +2592,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="13" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="1"/>
@@ -2226,7 +2613,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="1"/>
@@ -2434,7 +2821,7 @@
         <v>8</v>
       </c>
       <c r="M37" s="7" t="s">
-        <v>358</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -2455,7 +2842,7 @@
         <v>8</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>358</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -2476,7 +2863,7 @@
         <v>8</v>
       </c>
       <c r="M39" s="7" t="s">
-        <v>358</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
@@ -2497,7 +2884,7 @@
         <v>8</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>358</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
@@ -2518,7 +2905,7 @@
         <v>8</v>
       </c>
       <c r="M41" s="7" t="s">
-        <v>358</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -2538,6 +2925,9 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
+      <c r="M42" s="7" t="s">
+        <v>358</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2547,10 +2937,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F206"/>
+  <dimension ref="A1:F292"/>
   <sheetViews>
-    <sheetView topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="A196" sqref="A196:A206"/>
+    <sheetView topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162:A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2584,7 +2974,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1"/>
@@ -2600,7 +2990,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="1" t="s">
         <v>69</v>
       </c>
@@ -2616,7 +3006,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
@@ -2628,7 +3018,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="1" t="s">
         <v>73</v>
       </c>
@@ -2642,7 +3032,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
         <v>76</v>
       </c>
@@ -2658,7 +3048,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="1" t="s">
         <v>77</v>
       </c>
@@ -2672,7 +3062,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="1" t="s">
         <v>79</v>
       </c>
@@ -2686,7 +3076,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="1" t="s">
         <v>80</v>
       </c>
@@ -2700,7 +3090,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="1" t="s">
         <v>84</v>
       </c>
@@ -2714,7 +3104,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="1" t="s">
         <v>85</v>
       </c>
@@ -2728,7 +3118,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="1" t="s">
         <v>89</v>
       </c>
@@ -2742,7 +3132,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="1" t="s">
         <v>91</v>
       </c>
@@ -2756,7 +3146,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="1" t="s">
         <v>93</v>
       </c>
@@ -2770,7 +3160,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="1" t="s">
         <v>95</v>
       </c>
@@ -2784,7 +3174,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="1" t="s">
         <v>97</v>
       </c>
@@ -2798,7 +3188,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
@@ -2812,7 +3202,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="1" t="s">
         <v>103</v>
       </c>
@@ -2824,7 +3214,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="1" t="s">
         <v>104</v>
       </c>
@@ -2836,7 +3226,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="1" t="s">
         <v>105</v>
       </c>
@@ -2848,7 +3238,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="1" t="s">
         <v>106</v>
       </c>
@@ -2860,7 +3250,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="1" t="s">
         <v>107</v>
       </c>
@@ -2872,7 +3262,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="1" t="s">
         <v>108</v>
       </c>
@@ -2884,7 +3274,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="1" t="s">
         <v>109</v>
       </c>
@@ -2896,7 +3286,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="1" t="s">
         <v>60</v>
       </c>
@@ -2908,7 +3298,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="1" t="s">
         <v>110</v>
       </c>
@@ -2920,7 +3310,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="1" t="s">
         <v>111</v>
       </c>
@@ -2932,7 +3322,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="1" t="s">
         <v>112</v>
       </c>
@@ -2944,7 +3334,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="14" t="s">
         <v>53</v>
       </c>
       <c r="B29" s="1"/>
@@ -2956,7 +3346,7 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="1" t="s">
         <v>69</v>
       </c>
@@ -2970,7 +3360,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="1" t="s">
         <v>72</v>
       </c>
@@ -2984,7 +3374,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="1" t="s">
         <v>118</v>
       </c>
@@ -2998,7 +3388,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="5" t="s">
         <v>120</v>
       </c>
@@ -3012,7 +3402,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="14"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="1" t="s">
         <v>84</v>
       </c>
@@ -3026,7 +3416,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="1" t="s">
         <v>123</v>
       </c>
@@ -3040,7 +3430,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="1" t="s">
         <v>125</v>
       </c>
@@ -3054,7 +3444,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="1" t="s">
         <v>127</v>
       </c>
@@ -3068,7 +3458,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="1" t="s">
         <v>129</v>
       </c>
@@ -3082,7 +3472,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="14"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="1" t="s">
         <v>131</v>
       </c>
@@ -3096,7 +3486,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="14"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="1" t="s">
         <v>133</v>
       </c>
@@ -3110,7 +3500,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="14"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="1" t="s">
         <v>135</v>
       </c>
@@ -3124,7 +3514,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="14"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="1" t="s">
         <v>137</v>
       </c>
@@ -3138,7 +3528,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="14"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="1" t="s">
         <v>139</v>
       </c>
@@ -3152,7 +3542,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="14"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="1" t="s">
         <v>141</v>
       </c>
@@ -3166,7 +3556,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="14"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="1" t="s">
         <v>143</v>
       </c>
@@ -3180,7 +3570,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="14"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="1" t="s">
         <v>145</v>
       </c>
@@ -3194,7 +3584,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="14"/>
+      <c r="A47" s="15"/>
       <c r="B47" s="1" t="s">
         <v>147</v>
       </c>
@@ -3208,7 +3598,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="14"/>
+      <c r="A48" s="15"/>
       <c r="B48" s="1" t="s">
         <v>149</v>
       </c>
@@ -3222,7 +3612,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="14"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="1" t="s">
         <v>151</v>
       </c>
@@ -3236,7 +3626,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="14"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="1" t="s">
         <v>153</v>
       </c>
@@ -3250,7 +3640,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="14"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="1" t="s">
         <v>155</v>
       </c>
@@ -3264,7 +3654,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="14"/>
+      <c r="A52" s="15"/>
       <c r="B52" s="1" t="s">
         <v>157</v>
       </c>
@@ -3278,7 +3668,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="14"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="1" t="s">
         <v>159</v>
       </c>
@@ -3292,7 +3682,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="15"/>
+      <c r="A54" s="16"/>
       <c r="B54" s="1" t="s">
         <v>161</v>
       </c>
@@ -3306,7 +3696,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B55" s="1"/>
@@ -3320,7 +3710,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="14"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="1" t="s">
         <v>163</v>
       </c>
@@ -3332,7 +3722,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="14"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="1" t="s">
         <v>164</v>
       </c>
@@ -3344,7 +3734,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="14"/>
+      <c r="A58" s="15"/>
       <c r="B58" s="1" t="s">
         <v>165</v>
       </c>
@@ -3356,7 +3746,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="14"/>
+      <c r="A59" s="15"/>
       <c r="B59" s="1" t="s">
         <v>166</v>
       </c>
@@ -3368,7 +3758,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="15"/>
+      <c r="A60" s="16"/>
       <c r="B60" s="1" t="s">
         <v>167</v>
       </c>
@@ -3380,7 +3770,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B61" s="5"/>
@@ -3394,7 +3784,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="19"/>
+      <c r="A62" s="21"/>
       <c r="B62" s="5" t="s">
         <v>169</v>
       </c>
@@ -3406,7 +3796,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="19"/>
+      <c r="A63" s="21"/>
       <c r="B63" s="5" t="s">
         <v>170</v>
       </c>
@@ -3418,7 +3808,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="19"/>
+      <c r="A64" s="21"/>
       <c r="B64" s="5" t="s">
         <v>171</v>
       </c>
@@ -3430,7 +3820,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="19"/>
+      <c r="A65" s="21"/>
       <c r="B65" s="5" t="s">
         <v>172</v>
       </c>
@@ -3460,7 +3850,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B67" s="5"/>
@@ -3476,7 +3866,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A68" s="16"/>
+      <c r="A68" s="17"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
         <v>185</v>
@@ -3488,7 +3878,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="16"/>
+      <c r="A69" s="17"/>
       <c r="B69" s="5" t="s">
         <v>180</v>
       </c>
@@ -3500,7 +3890,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="16"/>
+      <c r="A70" s="17"/>
       <c r="B70" s="5" t="s">
         <v>181</v>
       </c>
@@ -3512,7 +3902,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="16"/>
+      <c r="A71" s="17"/>
       <c r="B71" s="5" t="s">
         <v>182</v>
       </c>
@@ -3526,7 +3916,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="16"/>
+      <c r="A72" s="17"/>
       <c r="B72" s="5" t="s">
         <v>186</v>
       </c>
@@ -3540,7 +3930,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="16"/>
+      <c r="A73" s="17"/>
       <c r="B73" s="5" t="s">
         <v>188</v>
       </c>
@@ -3552,7 +3942,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="16"/>
+      <c r="A74" s="17"/>
       <c r="B74" s="5" t="s">
         <v>189</v>
       </c>
@@ -3568,7 +3958,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A75" s="16"/>
+      <c r="A75" s="17"/>
       <c r="B75" s="5" t="s">
         <v>192</v>
       </c>
@@ -3584,7 +3974,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A76" s="16"/>
+      <c r="A76" s="17"/>
       <c r="B76" s="5" t="s">
         <v>195</v>
       </c>
@@ -3600,7 +3990,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="16"/>
+      <c r="A77" s="17"/>
       <c r="B77" s="5" t="s">
         <v>198</v>
       </c>
@@ -3614,7 +4004,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A78" s="16"/>
+      <c r="A78" s="17"/>
       <c r="B78" s="5" t="s">
         <v>200</v>
       </c>
@@ -3630,7 +4020,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="16"/>
+      <c r="A79" s="17"/>
       <c r="B79" s="5" t="s">
         <v>202</v>
       </c>
@@ -3646,7 +4036,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="16"/>
+      <c r="A80" s="17"/>
       <c r="B80" s="5" t="s">
         <v>205</v>
       </c>
@@ -3662,7 +4052,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A81" s="16"/>
+      <c r="A81" s="17"/>
       <c r="B81" s="5" t="s">
         <v>208</v>
       </c>
@@ -3678,7 +4068,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A82" s="13" t="s">
+      <c r="A82" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B82" s="5"/>
@@ -3694,7 +4084,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="15"/>
+      <c r="A83" s="16"/>
       <c r="B83" s="5" t="s">
         <v>291</v>
       </c>
@@ -3706,7 +4096,7 @@
       <c r="F83" s="8"/>
     </row>
     <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A84" s="20" t="s">
+      <c r="A84" s="23" t="s">
         <v>285</v>
       </c>
       <c r="B84" s="1"/>
@@ -3720,7 +4110,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A85" s="20"/>
+      <c r="A85" s="23"/>
       <c r="B85" s="1"/>
       <c r="C85" s="5" t="s">
         <v>219</v>
@@ -3734,7 +4124,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="20"/>
+      <c r="A86" s="23"/>
       <c r="B86" s="1"/>
       <c r="C86" s="5" t="s">
         <v>229</v>
@@ -3746,7 +4136,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A87" s="20"/>
+      <c r="A87" s="23"/>
       <c r="B87" s="1"/>
       <c r="C87" s="5" t="s">
         <v>282</v>
@@ -3758,7 +4148,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="20"/>
+      <c r="A88" s="23"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
         <v>284</v>
@@ -3770,7 +4160,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="20"/>
+      <c r="A89" s="23"/>
       <c r="B89" s="5" t="s">
         <v>180</v>
       </c>
@@ -3782,7 +4172,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="20"/>
+      <c r="A90" s="23"/>
       <c r="B90" s="5" t="s">
         <v>181</v>
       </c>
@@ -3794,7 +4184,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A91" s="20"/>
+      <c r="A91" s="23"/>
       <c r="B91" s="5" t="s">
         <v>230</v>
       </c>
@@ -3806,7 +4196,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A92" s="20"/>
+      <c r="A92" s="23"/>
       <c r="B92" s="11" t="s">
         <v>218</v>
       </c>
@@ -3820,7 +4210,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="20"/>
+      <c r="A93" s="23"/>
       <c r="B93" s="5" t="s">
         <v>9</v>
       </c>
@@ -3834,7 +4224,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="20"/>
+      <c r="A94" s="23"/>
       <c r="B94" s="5" t="s">
         <v>215</v>
       </c>
@@ -3848,7 +4238,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="20"/>
+      <c r="A95" s="23"/>
       <c r="B95" s="5" t="s">
         <v>216</v>
       </c>
@@ -3860,7 +4250,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="20"/>
+      <c r="A96" s="23"/>
       <c r="B96" s="5" t="s">
         <v>221</v>
       </c>
@@ -3874,7 +4264,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="20"/>
+      <c r="A97" s="23"/>
       <c r="B97" s="5" t="s">
         <v>223</v>
       </c>
@@ -3888,7 +4278,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="20"/>
+      <c r="A98" s="23"/>
       <c r="B98" s="5" t="s">
         <v>225</v>
       </c>
@@ -3902,7 +4292,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="20"/>
+      <c r="A99" s="23"/>
       <c r="B99" s="5" t="s">
         <v>227</v>
       </c>
@@ -3930,7 +4320,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="13" t="s">
+      <c r="A101" s="14" t="s">
         <v>59</v>
       </c>
       <c r="B101" s="5"/>
@@ -3944,7 +4334,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" s="14"/>
+      <c r="A102" s="15"/>
       <c r="B102" s="5" t="s">
         <v>287</v>
       </c>
@@ -3954,7 +4344,7 @@
       <c r="F102" s="8"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" s="14"/>
+      <c r="A103" s="15"/>
       <c r="B103" s="5" t="s">
         <v>288</v>
       </c>
@@ -3964,7 +4354,7 @@
       <c r="F103" s="8"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" s="15"/>
+      <c r="A104" s="16"/>
       <c r="B104" s="5" t="s">
         <v>289</v>
       </c>
@@ -3974,7 +4364,7 @@
       <c r="F104" s="8"/>
     </row>
     <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A105" s="20" t="s">
+      <c r="A105" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B105" s="1"/>
@@ -3990,7 +4380,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" s="20"/>
+      <c r="A106" s="23"/>
       <c r="B106" s="5" t="s">
         <v>233</v>
       </c>
@@ -4002,7 +4392,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107" s="20"/>
+      <c r="A107" s="23"/>
       <c r="B107" s="5" t="s">
         <v>234</v>
       </c>
@@ -4016,7 +4406,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="20" t="s">
+      <c r="A108" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B108" s="1"/>
@@ -4030,7 +4420,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" s="20"/>
+      <c r="A109" s="23"/>
       <c r="B109" s="5" t="s">
         <v>236</v>
       </c>
@@ -4044,7 +4434,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A110" s="20" t="s">
+      <c r="A110" s="23" t="s">
         <v>239</v>
       </c>
       <c r="B110" s="1"/>
@@ -4062,7 +4452,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A111" s="20"/>
+      <c r="A111" s="23"/>
       <c r="B111" s="5" t="s">
         <v>243</v>
       </c>
@@ -4076,7 +4466,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="20"/>
+      <c r="A112" s="23"/>
       <c r="B112" s="1" t="s">
         <v>245</v>
       </c>
@@ -4090,7 +4480,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" s="20"/>
+      <c r="A113" s="23"/>
       <c r="B113" s="5" t="s">
         <v>247</v>
       </c>
@@ -4102,7 +4492,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" s="20"/>
+      <c r="A114" s="23"/>
       <c r="B114" s="1" t="s">
         <v>248</v>
       </c>
@@ -4116,7 +4506,7 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" s="20"/>
+      <c r="A115" s="23"/>
       <c r="B115" s="5" t="s">
         <v>250</v>
       </c>
@@ -4130,7 +4520,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A116" s="20" t="s">
+      <c r="A116" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B116" s="1"/>
@@ -4144,7 +4534,7 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="20"/>
+      <c r="A117" s="23"/>
       <c r="B117" s="5" t="s">
         <v>253</v>
       </c>
@@ -4156,7 +4546,7 @@
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="20" t="s">
+      <c r="A118" s="23" t="s">
         <v>14</v>
       </c>
       <c r="B118" s="1"/>
@@ -4170,7 +4560,7 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="20"/>
+      <c r="A119" s="23"/>
       <c r="B119" s="5" t="s">
         <v>255</v>
       </c>
@@ -4182,7 +4572,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="20"/>
+      <c r="A120" s="23"/>
       <c r="B120" s="1" t="s">
         <v>256</v>
       </c>
@@ -4194,7 +4584,7 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="20"/>
+      <c r="A121" s="23"/>
       <c r="B121" s="5" t="s">
         <v>257</v>
       </c>
@@ -4208,7 +4598,7 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122" s="20"/>
+      <c r="A122" s="23"/>
       <c r="B122" s="1" t="s">
         <v>259</v>
       </c>
@@ -4222,7 +4612,7 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123" s="20" t="s">
+      <c r="A123" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B123" s="1"/>
@@ -4236,7 +4626,7 @@
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" s="20"/>
+      <c r="A124" s="23"/>
       <c r="B124" s="1" t="s">
         <v>262</v>
       </c>
@@ -4248,7 +4638,7 @@
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A125" s="20"/>
+      <c r="A125" s="23"/>
       <c r="B125" s="1" t="s">
         <v>256</v>
       </c>
@@ -4262,7 +4652,7 @@
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A126" s="20"/>
+      <c r="A126" s="23"/>
       <c r="B126" s="1" t="s">
         <v>257</v>
       </c>
@@ -4276,7 +4666,7 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127" s="20"/>
+      <c r="A127" s="23"/>
       <c r="B127" s="1" t="s">
         <v>259</v>
       </c>
@@ -4290,7 +4680,7 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" s="20"/>
+      <c r="A128" s="23"/>
       <c r="B128" s="1" t="s">
         <v>266</v>
       </c>
@@ -4304,7 +4694,7 @@
       </c>
     </row>
     <row r="129" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="13" t="s">
+      <c r="A129" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B129" s="1"/>
@@ -4320,7 +4710,7 @@
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A130" s="14"/>
+      <c r="A130" s="15"/>
       <c r="B130" s="1" t="s">
         <v>270</v>
       </c>
@@ -4334,7 +4724,7 @@
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A131" s="14"/>
+      <c r="A131" s="15"/>
       <c r="B131" s="1" t="s">
         <v>272</v>
       </c>
@@ -4346,7 +4736,7 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" s="14"/>
+      <c r="A132" s="15"/>
       <c r="B132" s="1" t="s">
         <v>125</v>
       </c>
@@ -4358,7 +4748,7 @@
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A133" s="14"/>
+      <c r="A133" s="15"/>
       <c r="B133" s="1" t="s">
         <v>273</v>
       </c>
@@ -4370,7 +4760,7 @@
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A134" s="14"/>
+      <c r="A134" s="15"/>
       <c r="B134" s="1" t="s">
         <v>274</v>
       </c>
@@ -4382,7 +4772,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A135" s="14"/>
+      <c r="A135" s="15"/>
       <c r="B135" s="1" t="s">
         <v>275</v>
       </c>
@@ -4394,7 +4784,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A136" s="14"/>
+      <c r="A136" s="15"/>
       <c r="B136" s="1" t="s">
         <v>276</v>
       </c>
@@ -4406,7 +4796,7 @@
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A137" s="14"/>
+      <c r="A137" s="15"/>
       <c r="B137" s="1" t="s">
         <v>277</v>
       </c>
@@ -4418,7 +4808,7 @@
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A138" s="14"/>
+      <c r="A138" s="15"/>
       <c r="B138" s="1" t="s">
         <v>278</v>
       </c>
@@ -4430,7 +4820,7 @@
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A139" s="15"/>
+      <c r="A139" s="16"/>
       <c r="B139" s="1" t="s">
         <v>279</v>
       </c>
@@ -4442,7 +4832,7 @@
       </c>
     </row>
     <row r="140" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="17" t="s">
+      <c r="A140" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B140" s="1"/>
@@ -4456,7 +4846,7 @@
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A141" s="18"/>
+      <c r="A141" s="20"/>
       <c r="B141" s="1" t="s">
         <v>281</v>
       </c>
@@ -4468,7 +4858,7 @@
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A142" s="13" t="s">
+      <c r="A142" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B142" s="1"/>
@@ -4482,7 +4872,7 @@
       </c>
     </row>
     <row r="143" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A143" s="14"/>
+      <c r="A143" s="15"/>
       <c r="B143" s="5" t="s">
         <v>20</v>
       </c>
@@ -4494,7 +4884,7 @@
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A144" s="14"/>
+      <c r="A144" s="15"/>
       <c r="B144" s="1" t="s">
         <v>21</v>
       </c>
@@ -4506,7 +4896,7 @@
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A145" s="14"/>
+      <c r="A145" s="15"/>
       <c r="B145" s="1" t="s">
         <v>22</v>
       </c>
@@ -4518,7 +4908,7 @@
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A146" s="14"/>
+      <c r="A146" s="15"/>
       <c r="B146" s="1" t="s">
         <v>23</v>
       </c>
@@ -4530,7 +4920,7 @@
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A147" s="14"/>
+      <c r="A147" s="15"/>
       <c r="B147" s="1" t="s">
         <v>24</v>
       </c>
@@ -4542,7 +4932,7 @@
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A148" s="14"/>
+      <c r="A148" s="15"/>
       <c r="B148" s="1" t="s">
         <v>25</v>
       </c>
@@ -4554,7 +4944,7 @@
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A149" s="14"/>
+      <c r="A149" s="15"/>
       <c r="B149" s="1" t="s">
         <v>26</v>
       </c>
@@ -4566,7 +4956,7 @@
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A150" s="14"/>
+      <c r="A150" s="15"/>
       <c r="B150" s="1" t="s">
         <v>32</v>
       </c>
@@ -4578,7 +4968,7 @@
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A151" s="14"/>
+      <c r="A151" s="15"/>
       <c r="B151" s="1" t="s">
         <v>33</v>
       </c>
@@ -4590,7 +4980,7 @@
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A152" s="14"/>
+      <c r="A152" s="15"/>
       <c r="B152" s="1" t="s">
         <v>35</v>
       </c>
@@ -4602,7 +4992,7 @@
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A153" s="14"/>
+      <c r="A153" s="15"/>
       <c r="B153" s="1" t="s">
         <v>36</v>
       </c>
@@ -4614,7 +5004,7 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A154" s="15"/>
+      <c r="A154" s="16"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
@@ -4624,7 +5014,7 @@
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A155" s="13" t="s">
+      <c r="A155" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B155" s="1"/>
@@ -4638,7 +5028,7 @@
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A156" s="14"/>
+      <c r="A156" s="15"/>
       <c r="B156" s="1" t="s">
         <v>30</v>
       </c>
@@ -4650,7 +5040,7 @@
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A157" s="14"/>
+      <c r="A157" s="15"/>
       <c r="B157" s="1" t="s">
         <v>37</v>
       </c>
@@ -4662,7 +5052,7 @@
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A158" s="14"/>
+      <c r="A158" s="15"/>
       <c r="B158" s="1" t="s">
         <v>40</v>
       </c>
@@ -4674,7 +5064,7 @@
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A159" s="14"/>
+      <c r="A159" s="15"/>
       <c r="B159" s="1" t="s">
         <v>41</v>
       </c>
@@ -4688,7 +5078,7 @@
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A160" s="14"/>
+      <c r="A160" s="15"/>
       <c r="B160" s="1" t="s">
         <v>39</v>
       </c>
@@ -4702,7 +5092,7 @@
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A161" s="15"/>
+      <c r="A161" s="16"/>
       <c r="B161" s="1" t="s">
         <v>43</v>
       </c>
@@ -4714,7 +5104,7 @@
       </c>
     </row>
     <row r="162" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A162" s="13" t="s">
+      <c r="A162" s="14" t="s">
         <v>45</v>
       </c>
       <c r="B162" s="1"/>
@@ -4732,7 +5122,7 @@
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A163" s="15"/>
+      <c r="A163" s="16"/>
       <c r="B163" s="1" t="s">
         <v>349</v>
       </c>
@@ -4744,7 +5134,7 @@
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A164" s="21" t="s">
+      <c r="A164" s="18" t="s">
         <v>350</v>
       </c>
       <c r="B164" s="9" t="s">
@@ -4764,7 +5154,7 @@
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A165" s="22"/>
+      <c r="A165" s="19"/>
       <c r="B165" s="9" t="s">
         <v>47</v>
       </c>
@@ -4782,7 +5172,7 @@
       </c>
     </row>
     <row r="166" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A166" s="22"/>
+      <c r="A166" s="19"/>
       <c r="B166" s="9" t="s">
         <v>300</v>
       </c>
@@ -4800,7 +5190,7 @@
       </c>
     </row>
     <row r="167" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A167" s="18"/>
+      <c r="A167" s="20"/>
       <c r="B167" s="9" t="s">
         <v>49</v>
       </c>
@@ -4890,7 +5280,7 @@
       </c>
     </row>
     <row r="173" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A173" s="13" t="s">
+      <c r="A173" s="14" t="s">
         <v>315</v>
       </c>
       <c r="B173" s="1"/>
@@ -4904,7 +5294,7 @@
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A174" s="14"/>
+      <c r="A174" s="15"/>
       <c r="B174" s="1" t="s">
         <v>287</v>
       </c>
@@ -4916,7 +5306,7 @@
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A175" s="14"/>
+      <c r="A175" s="15"/>
       <c r="B175" s="1" t="s">
         <v>288</v>
       </c>
@@ -4928,7 +5318,7 @@
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A176" s="14"/>
+      <c r="A176" s="15"/>
       <c r="B176" s="1" t="s">
         <v>256</v>
       </c>
@@ -4940,7 +5330,7 @@
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A177" s="14"/>
+      <c r="A177" s="15"/>
       <c r="B177" s="1" t="s">
         <v>317</v>
       </c>
@@ -4952,7 +5342,7 @@
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A178" s="15"/>
+      <c r="A178" s="16"/>
       <c r="B178" s="1" t="s">
         <v>318</v>
       </c>
@@ -4964,7 +5354,7 @@
       </c>
     </row>
     <row r="179" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A179" s="16" t="s">
+      <c r="A179" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B179" s="5"/>
@@ -4978,7 +5368,7 @@
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A180" s="16"/>
+      <c r="A180" s="17"/>
       <c r="B180" s="5" t="s">
         <v>69</v>
       </c>
@@ -4990,7 +5380,7 @@
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A181" s="16"/>
+      <c r="A181" s="17"/>
       <c r="B181" s="5" t="s">
         <v>72</v>
       </c>
@@ -5002,7 +5392,7 @@
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A182" s="16"/>
+      <c r="A182" s="17"/>
       <c r="B182" s="5" t="s">
         <v>176</v>
       </c>
@@ -5014,7 +5404,7 @@
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A183" s="16"/>
+      <c r="A183" s="17"/>
       <c r="B183" s="5" t="s">
         <v>177</v>
       </c>
@@ -5026,7 +5416,7 @@
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A184" s="16"/>
+      <c r="A184" s="17"/>
       <c r="B184" s="5" t="s">
         <v>178</v>
       </c>
@@ -5038,7 +5428,7 @@
       </c>
     </row>
     <row r="185" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A185" s="13" t="s">
+      <c r="A185" s="14" t="s">
         <v>60</v>
       </c>
       <c r="B185" s="1"/>
@@ -5052,7 +5442,7 @@
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A186" s="14"/>
+      <c r="A186" s="15"/>
       <c r="B186" s="8" t="s">
         <v>60</v>
       </c>
@@ -5066,7 +5456,7 @@
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A187" s="14"/>
+      <c r="A187" s="15"/>
       <c r="B187" s="8" t="s">
         <v>322</v>
       </c>
@@ -5080,7 +5470,7 @@
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A188" s="14"/>
+      <c r="A188" s="15"/>
       <c r="B188" s="8" t="s">
         <v>288</v>
       </c>
@@ -5094,7 +5484,7 @@
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A189" s="14"/>
+      <c r="A189" s="15"/>
       <c r="B189" s="8" t="s">
         <v>325</v>
       </c>
@@ -5108,7 +5498,7 @@
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A190" s="14"/>
+      <c r="A190" s="15"/>
       <c r="B190" s="8" t="s">
         <v>327</v>
       </c>
@@ -5122,7 +5512,7 @@
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A191" s="14"/>
+      <c r="A191" s="15"/>
       <c r="B191" s="8" t="s">
         <v>329</v>
       </c>
@@ -5136,7 +5526,7 @@
       </c>
     </row>
     <row r="192" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A192" s="14"/>
+      <c r="A192" s="15"/>
       <c r="B192" s="8" t="s">
         <v>331</v>
       </c>
@@ -5150,7 +5540,7 @@
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A193" s="14"/>
+      <c r="A193" s="15"/>
       <c r="B193" s="8" t="s">
         <v>333</v>
       </c>
@@ -5164,7 +5554,7 @@
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A194" s="14"/>
+      <c r="A194" s="15"/>
       <c r="B194" s="8" t="s">
         <v>335</v>
       </c>
@@ -5178,7 +5568,7 @@
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A195" s="15"/>
+      <c r="A195" s="16"/>
       <c r="B195" s="8" t="s">
         <v>337</v>
       </c>
@@ -5192,7 +5582,7 @@
       </c>
     </row>
     <row r="196" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A196" s="13" t="s">
+      <c r="A196" s="14" t="s">
         <v>61</v>
       </c>
       <c r="B196" s="1"/>
@@ -5206,7 +5596,7 @@
       </c>
     </row>
     <row r="197" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A197" s="14"/>
+      <c r="A197" s="15"/>
       <c r="B197" s="8" t="s">
         <v>60</v>
       </c>
@@ -5220,7 +5610,7 @@
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A198" s="14"/>
+      <c r="A198" s="15"/>
       <c r="B198" s="8" t="s">
         <v>61</v>
       </c>
@@ -5234,7 +5624,7 @@
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A199" s="14"/>
+      <c r="A199" s="15"/>
       <c r="B199" s="8" t="s">
         <v>288</v>
       </c>
@@ -5248,7 +5638,7 @@
       </c>
     </row>
     <row r="200" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A200" s="14"/>
+      <c r="A200" s="15"/>
       <c r="B200" s="8" t="s">
         <v>331</v>
       </c>
@@ -5262,7 +5652,7 @@
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A201" s="14"/>
+      <c r="A201" s="15"/>
       <c r="B201" s="8" t="s">
         <v>344</v>
       </c>
@@ -5276,7 +5666,7 @@
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A202" s="14"/>
+      <c r="A202" s="15"/>
       <c r="B202" s="8" t="s">
         <v>346</v>
       </c>
@@ -5290,7 +5680,7 @@
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A203" s="14"/>
+      <c r="A203" s="15"/>
       <c r="B203" s="8" t="s">
         <v>351</v>
       </c>
@@ -5304,7 +5694,7 @@
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A204" s="14"/>
+      <c r="A204" s="15"/>
       <c r="B204" s="8" t="s">
         <v>353</v>
       </c>
@@ -5318,7 +5708,7 @@
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A205" s="14"/>
+      <c r="A205" s="15"/>
       <c r="B205" s="8" t="s">
         <v>355</v>
       </c>
@@ -5332,7 +5722,7 @@
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A206" s="15"/>
+      <c r="A206" s="16"/>
       <c r="B206" s="8" t="s">
         <v>111</v>
       </c>
@@ -5345,14 +5735,1219 @@
         <v>14</v>
       </c>
     </row>
+    <row r="207" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A207" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B207" s="1"/>
+      <c r="C207" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="D207" s="1"/>
+      <c r="E207" s="1"/>
+      <c r="F207" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A208" s="23"/>
+      <c r="B208" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C208" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="D208" s="1"/>
+      <c r="E208" s="1"/>
+      <c r="F208" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A209" s="23"/>
+      <c r="B209" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C209" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="D209" s="1"/>
+      <c r="E209" s="1"/>
+      <c r="F209" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A210" s="23"/>
+      <c r="B210" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="C210" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="D210" s="1"/>
+      <c r="E210" s="1"/>
+      <c r="F210" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A211" s="23"/>
+      <c r="B211" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C211" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="D211" s="1"/>
+      <c r="E211" s="1"/>
+      <c r="F211" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A212" s="23"/>
+      <c r="B212" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="C212" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="D212" s="1"/>
+      <c r="E212" s="1"/>
+      <c r="F212" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A213" s="23"/>
+      <c r="B213" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C213" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D213" s="1"/>
+      <c r="E213" s="1"/>
+      <c r="F213" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A214" s="23"/>
+      <c r="B214" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="C214" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="D214" s="1"/>
+      <c r="E214" s="1"/>
+      <c r="F214" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A215" s="23"/>
+      <c r="B215" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="C215" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D215" s="1"/>
+      <c r="E215" s="1"/>
+      <c r="F215" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A216" s="23"/>
+      <c r="B216" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="C216" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="D216" s="1"/>
+      <c r="E216" s="1"/>
+      <c r="F216" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A217" s="23"/>
+      <c r="B217" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="C217" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="D217" s="1"/>
+      <c r="E217" s="1"/>
+      <c r="F217" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A218" s="23"/>
+      <c r="B218" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="C218" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="D218" s="1"/>
+      <c r="E218" s="1"/>
+      <c r="F218" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A219" s="23"/>
+      <c r="B219" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="C219" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="D219" s="1"/>
+      <c r="E219" s="1"/>
+      <c r="F219" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A220" s="23"/>
+      <c r="B220" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="C220" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="D220" s="1"/>
+      <c r="E220" s="1"/>
+      <c r="F220" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A221" s="23"/>
+      <c r="B221" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="C221" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D221" s="1"/>
+      <c r="E221" s="1"/>
+      <c r="F221" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A222" s="23"/>
+      <c r="B222" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="C222" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="D222" s="1"/>
+      <c r="E222" s="1"/>
+      <c r="F222" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A223" s="23"/>
+      <c r="B223" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="C223" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="D223" s="1"/>
+      <c r="E223" s="1"/>
+      <c r="F223" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A224" s="23"/>
+      <c r="B224" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="C224" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="D224" s="1"/>
+      <c r="E224" s="1"/>
+      <c r="F224" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A225" s="23"/>
+      <c r="B225" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="C225" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="D225" s="1"/>
+      <c r="E225" s="1"/>
+      <c r="F225" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A226" s="23"/>
+      <c r="B226" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C226" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="D226" s="1"/>
+      <c r="E226" s="1"/>
+      <c r="F226" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A227" s="23"/>
+      <c r="B227" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="C227" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="D227" s="1"/>
+      <c r="E227" s="1"/>
+      <c r="F227" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B228" s="1"/>
+      <c r="C228" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="D228" s="1"/>
+      <c r="E228" s="1"/>
+      <c r="F228" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A229" s="23"/>
+      <c r="B229" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C229" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="D229" s="1"/>
+      <c r="E229" s="1"/>
+      <c r="F229" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A230" s="23"/>
+      <c r="B230" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C230" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="D230" s="1"/>
+      <c r="E230" s="1"/>
+      <c r="F230" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A231" s="23"/>
+      <c r="B231" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="C231" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="D231" s="1"/>
+      <c r="E231" s="1"/>
+      <c r="F231" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A232" s="23"/>
+      <c r="B232" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C232" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="D232" s="1"/>
+      <c r="E232" s="1"/>
+      <c r="F232" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A233" s="23"/>
+      <c r="B233" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="C233" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="D233" s="1"/>
+      <c r="E233" s="1"/>
+      <c r="F233" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A234" s="23"/>
+      <c r="B234" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="C234" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="D234" s="1"/>
+      <c r="E234" s="1"/>
+      <c r="F234" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A235" s="23"/>
+      <c r="B235" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="C235" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="D235" s="1"/>
+      <c r="E235" s="1"/>
+      <c r="F235" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A236" s="23"/>
+      <c r="B236" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C236" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="D236" s="1"/>
+      <c r="E236" s="1"/>
+      <c r="F236" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A237" s="23"/>
+      <c r="B237" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="C237" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D237" s="1"/>
+      <c r="E237" s="1"/>
+      <c r="F237" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A238" s="23"/>
+      <c r="B238" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="C238" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="D238" s="1"/>
+      <c r="E238" s="1"/>
+      <c r="F238" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A239" s="23"/>
+      <c r="B239" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="C239" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="D239" s="1"/>
+      <c r="E239" s="1"/>
+      <c r="F239" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A240" s="23"/>
+      <c r="B240" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="C240" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="D240" s="1"/>
+      <c r="E240" s="1"/>
+      <c r="F240" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A241" s="23"/>
+      <c r="B241" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="C241" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="D241" s="1"/>
+      <c r="E241" s="1"/>
+      <c r="F241" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A242" s="23"/>
+      <c r="B242" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="C242" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="D242" s="1"/>
+      <c r="E242" s="1"/>
+      <c r="F242" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A243" s="23"/>
+      <c r="B243" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="C243" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="D243" s="1"/>
+      <c r="E243" s="1"/>
+      <c r="F243" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A244" s="23"/>
+      <c r="B244" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="C244" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="D244" s="1"/>
+      <c r="E244" s="1"/>
+      <c r="F244" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A245" s="23"/>
+      <c r="B245" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C245" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="D245" s="1"/>
+      <c r="E245" s="1"/>
+      <c r="F245" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A246" s="23"/>
+      <c r="B246" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="C246" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="D246" s="1"/>
+      <c r="E246" s="1"/>
+      <c r="F246" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A247" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B247" s="1"/>
+      <c r="C247" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="D247" s="1"/>
+      <c r="E247" s="1"/>
+      <c r="F247" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A248" s="24"/>
+      <c r="B248" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C248" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="D248" s="1"/>
+      <c r="E248" s="1"/>
+      <c r="F248" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A249" s="24"/>
+      <c r="B249" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C249" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="D249" s="1"/>
+      <c r="E249" s="1"/>
+      <c r="F249" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A250" s="24"/>
+      <c r="B250" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="C250" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="D250" s="1"/>
+      <c r="E250" s="1"/>
+      <c r="F250" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A251" s="24"/>
+      <c r="B251" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C251" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="D251" s="1"/>
+      <c r="E251" s="1"/>
+      <c r="F251" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A252" s="24"/>
+      <c r="B252" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="C252" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="D252" s="1"/>
+      <c r="E252" s="1"/>
+      <c r="F252" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A253" s="24"/>
+      <c r="B253" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="C253" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D253" s="1"/>
+      <c r="E253" s="1"/>
+      <c r="F253" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A254" s="24"/>
+      <c r="B254" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="C254" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="D254" s="1"/>
+      <c r="E254" s="1"/>
+      <c r="F254" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A255" s="24"/>
+      <c r="B255" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C255" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="D255" s="1"/>
+      <c r="E255" s="1"/>
+      <c r="F255" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A256" s="24"/>
+      <c r="B256" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="C256" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="D256" s="1"/>
+      <c r="E256" s="1"/>
+      <c r="F256" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A257" s="24"/>
+      <c r="B257" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="C257" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="D257" s="1"/>
+      <c r="E257" s="1"/>
+      <c r="F257" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A258" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B258" s="1"/>
+      <c r="C258" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="D258" s="1"/>
+      <c r="E258" s="1"/>
+      <c r="F258" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A259" s="23"/>
+      <c r="B259" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C259" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="D259" s="1"/>
+      <c r="E259" s="1"/>
+      <c r="F259" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A260" s="23"/>
+      <c r="B260" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C260" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="D260" s="1"/>
+      <c r="E260" s="1"/>
+      <c r="F260" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A261" s="23"/>
+      <c r="B261" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="C261" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="D261" s="1"/>
+      <c r="E261" s="1"/>
+      <c r="F261" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A262" s="23"/>
+      <c r="B262" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C262" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="D262" s="1"/>
+      <c r="E262" s="1"/>
+      <c r="F262" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A263" s="23"/>
+      <c r="B263" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="C263" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="D263" s="1"/>
+      <c r="E263" s="1"/>
+      <c r="F263" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A264" s="23"/>
+      <c r="B264" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="C264" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="D264" s="1"/>
+      <c r="E264" s="1"/>
+      <c r="F264" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A265" s="23"/>
+      <c r="B265" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="C265" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="D265" s="1"/>
+      <c r="E265" s="1"/>
+      <c r="F265" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A266" s="23"/>
+      <c r="B266" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C266" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="D266" s="1"/>
+      <c r="E266" s="1"/>
+      <c r="F266" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A267" s="23"/>
+      <c r="B267" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="C267" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D267" s="1"/>
+      <c r="E267" s="1"/>
+      <c r="F267" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A268" s="23"/>
+      <c r="B268" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="C268" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="D268" s="1"/>
+      <c r="E268" s="1"/>
+      <c r="F268" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A269" s="23"/>
+      <c r="B269" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="C269" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="D269" s="1"/>
+      <c r="E269" s="1"/>
+      <c r="F269" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A270" s="23"/>
+      <c r="B270" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="C270" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="D270" s="1"/>
+      <c r="E270" s="1"/>
+      <c r="F270" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A271" s="23"/>
+      <c r="B271" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="C271" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="D271" s="1"/>
+      <c r="E271" s="1"/>
+      <c r="F271" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A272" s="23"/>
+      <c r="B272" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="C272" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="D272" s="1"/>
+      <c r="E272" s="1"/>
+      <c r="F272" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A273" s="23"/>
+      <c r="B273" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="C273" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="D273" s="1"/>
+      <c r="E273" s="1"/>
+      <c r="F273" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A274" s="23"/>
+      <c r="B274" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="C274" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="D274" s="1"/>
+      <c r="E274" s="1"/>
+      <c r="F274" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A275" s="23"/>
+      <c r="B275" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C275" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D275" s="1"/>
+      <c r="E275" s="1"/>
+      <c r="F275" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A276" s="23"/>
+      <c r="B276" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="C276" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="D276" s="1"/>
+      <c r="E276" s="1"/>
+      <c r="F276" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A277" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B277" s="1"/>
+      <c r="C277" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="D277" s="1"/>
+      <c r="E277" s="1"/>
+      <c r="F277" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A278" s="23"/>
+      <c r="B278" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C278" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="D278" s="1"/>
+      <c r="E278" s="1"/>
+      <c r="F278" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A279" s="23"/>
+      <c r="B279" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C279" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="D279" s="1"/>
+      <c r="E279" s="1"/>
+      <c r="F279" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A280" s="23"/>
+      <c r="B280" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="C280" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="D280" s="1"/>
+      <c r="E280" s="1"/>
+      <c r="F280" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A281" s="23"/>
+      <c r="B281" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="C281" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="D281" s="1"/>
+      <c r="E281" s="1"/>
+      <c r="F281" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A282" s="23"/>
+      <c r="B282" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="C282" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="D282" s="1"/>
+      <c r="E282" s="1"/>
+      <c r="F282" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A283" s="23"/>
+      <c r="B283" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="C283" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="D283" s="1"/>
+      <c r="E283" s="1"/>
+      <c r="F283" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A284" s="23"/>
+      <c r="B284" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C284" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="D284" s="1"/>
+      <c r="E284" s="1"/>
+      <c r="F284" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A285" s="23"/>
+      <c r="B285" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="C285" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="D285" s="1"/>
+      <c r="E285" s="1"/>
+      <c r="F285" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A286" s="23"/>
+      <c r="B286" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="C286" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="D286" s="1"/>
+      <c r="E286" s="1"/>
+      <c r="F286" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A287" s="23"/>
+      <c r="B287" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="C287" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="D287" s="1"/>
+      <c r="E287" s="1"/>
+      <c r="F287" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A288" s="23"/>
+      <c r="B288" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="C288" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="D288" s="1"/>
+      <c r="E288" s="1"/>
+      <c r="F288" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A289" s="23"/>
+      <c r="B289" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="C289" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="D289" s="1"/>
+      <c r="E289" s="1"/>
+      <c r="F289" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A290" s="23"/>
+      <c r="B290" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="C290" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D290" s="1"/>
+      <c r="E290" s="1"/>
+      <c r="F290" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A291" s="23"/>
+      <c r="B291" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="C291" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="D291" s="1"/>
+      <c r="E291" s="1"/>
+      <c r="F291" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A292" s="23"/>
+      <c r="B292" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="C292" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="D292" s="1"/>
+      <c r="E292" s="1"/>
+      <c r="F292" s="8">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A185:A195"/>
-    <mergeCell ref="A196:A206"/>
-    <mergeCell ref="A173:A178"/>
-    <mergeCell ref="A179:A184"/>
-    <mergeCell ref="A162:A163"/>
-    <mergeCell ref="A164:A167"/>
+  <mergeCells count="29">
+    <mergeCell ref="A258:A276"/>
+    <mergeCell ref="A277:A292"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A207:A227"/>
+    <mergeCell ref="A228:A246"/>
+    <mergeCell ref="A247:A257"/>
     <mergeCell ref="A2:A28"/>
     <mergeCell ref="A29:A54"/>
     <mergeCell ref="A55:A60"/>
@@ -5369,8 +6964,12 @@
     <mergeCell ref="A105:A107"/>
     <mergeCell ref="A108:A109"/>
     <mergeCell ref="A110:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A185:A195"/>
+    <mergeCell ref="A196:A206"/>
+    <mergeCell ref="A173:A178"/>
+    <mergeCell ref="A179:A184"/>
+    <mergeCell ref="A162:A163"/>
+    <mergeCell ref="A164:A167"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1"/>

</xml_diff>

<commit_message>
update from notes taken during the webconf
</commit_message>
<xml_diff>
--- a/Vocabulary/BoreholeIE_consolidated_vocab.xlsx
+++ b/Vocabulary/BoreholeIE_consolidated_vocab.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="535">
   <si>
     <t>Concept</t>
   </si>
@@ -1647,12 +1647,6 @@
     <t>Borehole/boreholeShape</t>
   </si>
   <si>
-    <t>outerRim of BhML, more a reuse of standardized description of Borehole Logs</t>
-  </si>
-  <si>
-    <t>? O&amp;M on core (on Sample ?) or also on other features (Borehole) ?</t>
-  </si>
-  <si>
     <t>DrillingCampaign and DrillingOperation</t>
   </si>
   <si>
@@ -1669,6 +1663,15 @@
   </si>
   <si>
     <t>BhML:Sample as well with recursive link ?</t>
+  </si>
+  <si>
+    <t>Feature observed in Borehole Log.</t>
+  </si>
+  <si>
+    <t>outerRim of BhML, more a reuse of standardized description of Borehole Logs -&gt; may need to create a GitHub issue on this</t>
+  </si>
+  <si>
+    <t>? O&amp;M on core (on Sample ?) or also on other features (Borehole) ? -&gt; clarified during webconf 15</t>
   </si>
 </sst>
 </file>
@@ -1803,7 +1806,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1835,39 +1838,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1882,9 +1852,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1906,18 +1873,63 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2204,7 +2216,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2214,7 +2226,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="19" t="s">
         <v>509</v>
       </c>
       <c r="B1" t="s">
@@ -2222,18 +2234,18 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="19" t="s">
         <v>510</v>
       </c>
       <c r="B2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="19" t="s">
         <v>512</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="20" t="s">
         <v>513</v>
       </c>
     </row>
@@ -2247,93 +2259,93 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.44140625" customWidth="1"/>
-    <col min="13" max="13" width="44.33203125" style="26" customWidth="1"/>
+    <col min="13" max="13" width="44.33203125" style="15" customWidth="1"/>
     <col min="14" max="14" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="38">
+      <c r="C1" s="26">
         <v>2</v>
       </c>
-      <c r="D1" s="38">
+      <c r="D1" s="26">
         <v>3</v>
       </c>
-      <c r="E1" s="38">
+      <c r="E1" s="26">
         <v>4</v>
       </c>
-      <c r="F1" s="38">
+      <c r="F1" s="26">
         <v>5</v>
       </c>
-      <c r="G1" s="38">
+      <c r="G1" s="26">
         <v>6</v>
       </c>
-      <c r="H1" s="38">
+      <c r="H1" s="26">
         <v>7</v>
       </c>
-      <c r="I1" s="38">
-        <v>8</v>
-      </c>
-      <c r="J1" s="38">
+      <c r="I1" s="26">
+        <v>8</v>
+      </c>
+      <c r="J1" s="26">
         <v>11</v>
       </c>
-      <c r="K1" s="38">
+      <c r="K1" s="26">
         <v>13</v>
       </c>
-      <c r="L1" s="38">
-        <v>14</v>
-      </c>
-      <c r="M1" s="40" t="s">
+      <c r="L1" s="26">
+        <v>14</v>
+      </c>
+      <c r="M1" s="28" t="s">
         <v>506</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="27" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="37" t="s">
+      <c r="B2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="25" t="s">
         <v>3</v>
       </c>
       <c r="N2" s="6" t="s">
@@ -2357,7 +2369,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="21" t="s">
         <v>503</v>
       </c>
       <c r="N3" s="6" t="s">
@@ -2381,7 +2393,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="32" t="s">
+      <c r="M4" s="21" t="s">
         <v>504</v>
       </c>
       <c r="N4" s="6" t="s">
@@ -2405,7 +2417,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="21" t="s">
         <v>505</v>
       </c>
       <c r="N5" s="6" t="s">
@@ -2429,7 +2441,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="32" t="s">
+      <c r="M6" s="21" t="s">
         <v>507</v>
       </c>
       <c r="N6" s="6" t="s">
@@ -2457,7 +2469,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="33" t="s">
+      <c r="M7" s="22" t="s">
         <v>519</v>
       </c>
       <c r="N7" s="6" t="s">
@@ -2481,7 +2493,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="32" t="s">
+      <c r="M8" s="21" t="s">
         <v>508</v>
       </c>
       <c r="N8" s="6" t="s">
@@ -2489,29 +2501,29 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="34" t="s">
+      <c r="B9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="32" t="s">
         <v>514</v>
       </c>
       <c r="N9" s="6" t="s">
@@ -2519,89 +2531,89 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="34"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="32"/>
       <c r="N10" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="34"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="32"/>
       <c r="N11" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="34"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="32"/>
       <c r="N12" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="L13" s="29"/>
-      <c r="M13" s="34"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" s="18"/>
+      <c r="M13" s="32"/>
       <c r="N13" s="6" t="s">
         <v>8</v>
       </c>
@@ -2623,7 +2635,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="32" t="s">
+      <c r="M14" s="21" t="s">
         <v>517</v>
       </c>
       <c r="N14" s="6" t="s">
@@ -2647,7 +2659,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="32" t="s">
+      <c r="M15" s="21" t="s">
         <v>517</v>
       </c>
       <c r="N15" s="6" t="s">
@@ -2671,7 +2683,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="33" t="s">
+      <c r="M16" s="22" t="s">
         <v>515</v>
       </c>
       <c r="N16" s="6" t="s">
@@ -2695,7 +2707,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="33" t="s">
+      <c r="M17" s="22" t="s">
         <v>518</v>
       </c>
       <c r="N17" s="6" t="s">
@@ -2719,7 +2731,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="32" t="s">
+      <c r="M18" s="21" t="s">
         <v>520</v>
       </c>
       <c r="N18" s="6" t="s">
@@ -2743,7 +2755,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="32" t="s">
+      <c r="M19" s="21" t="s">
         <v>521</v>
       </c>
       <c r="N19" s="6" t="s">
@@ -2767,7 +2779,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="41" t="s">
+      <c r="M20" s="33" t="s">
         <v>516</v>
       </c>
       <c r="N20" s="6" t="s">
@@ -2791,7 +2803,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="42"/>
+      <c r="M21" s="34"/>
       <c r="N21" s="6" t="s">
         <v>8</v>
       </c>
@@ -2813,7 +2825,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="33" t="s">
+      <c r="M22" s="22" t="s">
         <v>523</v>
       </c>
       <c r="N22" s="6" t="s">
@@ -2835,7 +2847,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="32" t="s">
+      <c r="M23" s="21" t="s">
         <v>522</v>
       </c>
       <c r="N23" s="6" t="s">
@@ -2859,7 +2871,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-      <c r="M24" s="32" t="s">
+      <c r="M24" s="21" t="s">
         <v>525</v>
       </c>
       <c r="N24" s="6" t="s">
@@ -2867,23 +2879,23 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="43" t="s">
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="30" t="s">
         <v>524</v>
       </c>
       <c r="N25" s="6" t="s">
@@ -2891,67 +2903,67 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="44"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="35"/>
       <c r="N26" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="44"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="35"/>
       <c r="N27" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="45"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="31"/>
       <c r="N28" s="6" t="s">
         <v>8</v>
       </c>
@@ -2973,8 +2985,8 @@
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="43" t="s">
-        <v>526</v>
+      <c r="M29" s="29" t="s">
+        <v>532</v>
       </c>
       <c r="N29" s="6" t="s">
         <v>8</v>
@@ -2997,7 +3009,9 @@
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="44"/>
+      <c r="M30" s="30" t="s">
+        <v>533</v>
+      </c>
       <c r="N30" s="6" t="s">
         <v>8</v>
       </c>
@@ -3019,7 +3033,7 @@
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-      <c r="M31" s="44"/>
+      <c r="M31" s="47"/>
       <c r="N31" s="6" t="s">
         <v>8</v>
       </c>
@@ -3041,7 +3055,7 @@
       </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="45"/>
+      <c r="M32" s="48"/>
       <c r="N32" s="6" t="s">
         <v>8</v>
       </c>
@@ -3063,80 +3077,80 @@
         <v>8</v>
       </c>
       <c r="L33" s="1"/>
-      <c r="M33" s="33" t="s">
+      <c r="M33" s="22" t="s">
+        <v>534</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M34" s="30" t="s">
+        <v>526</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M35" s="31"/>
+      <c r="N35" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M36" s="21" t="s">
         <v>527</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
-      <c r="L34" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="M34" s="43" t="s">
-        <v>528</v>
-      </c>
-      <c r="N34" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="M35" s="45"/>
-      <c r="N35" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
-      <c r="L36" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="M36" s="32" t="s">
-        <v>529</v>
       </c>
       <c r="N36" s="6" t="s">
         <v>8</v>
@@ -3159,8 +3173,8 @@
       <c r="L37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M37" s="32" t="s">
-        <v>530</v>
+      <c r="M37" s="21" t="s">
+        <v>528</v>
       </c>
       <c r="N37" s="6" t="s">
         <v>8</v>
@@ -3183,8 +3197,8 @@
       <c r="L38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M38" s="43" t="s">
-        <v>533</v>
+      <c r="M38" s="30" t="s">
+        <v>531</v>
       </c>
       <c r="N38" s="6" t="s">
         <v>8</v>
@@ -3207,7 +3221,7 @@
       <c r="L39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M39" s="45"/>
+      <c r="M39" s="31"/>
       <c r="N39" s="6" t="s">
         <v>8</v>
       </c>
@@ -3229,8 +3243,8 @@
       <c r="L40" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M40" s="32" t="s">
-        <v>532</v>
+      <c r="M40" s="21" t="s">
+        <v>530</v>
       </c>
       <c r="N40" s="6" t="s">
         <v>8</v>
@@ -3253,8 +3267,8 @@
       <c r="L41" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="32" t="s">
-        <v>529</v>
+      <c r="M41" s="21" t="s">
+        <v>527</v>
       </c>
       <c r="N41" s="6" t="s">
         <v>8</v>
@@ -3288,8 +3302,8 @@
     <mergeCell ref="M9:M13"/>
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="M25:M28"/>
-    <mergeCell ref="M29:M32"/>
     <mergeCell ref="M34:M35"/>
+    <mergeCell ref="M30:M32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3300,8 +3314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F292"/>
   <sheetViews>
-    <sheetView topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="C247" sqref="C247"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="C168" sqref="C168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3335,7 +3349,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="37" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1"/>
@@ -3351,7 +3365,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="1" t="s">
         <v>69</v>
       </c>
@@ -3367,7 +3381,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
@@ -3379,7 +3393,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="1" t="s">
         <v>73</v>
       </c>
@@ -3393,7 +3407,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="1" t="s">
         <v>76</v>
       </c>
@@ -3409,7 +3423,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="1" t="s">
         <v>77</v>
       </c>
@@ -3423,7 +3437,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="1" t="s">
         <v>79</v>
       </c>
@@ -3437,7 +3451,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="1" t="s">
         <v>80</v>
       </c>
@@ -3451,7 +3465,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="1" t="s">
         <v>84</v>
       </c>
@@ -3465,7 +3479,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="1" t="s">
         <v>85</v>
       </c>
@@ -3479,7 +3493,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="1" t="s">
         <v>89</v>
       </c>
@@ -3493,7 +3507,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="1" t="s">
         <v>91</v>
       </c>
@@ -3507,7 +3521,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="1" t="s">
         <v>93</v>
       </c>
@@ -3521,7 +3535,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="1" t="s">
         <v>95</v>
       </c>
@@ -3535,7 +3549,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="1" t="s">
         <v>97</v>
       </c>
@@ -3549,7 +3563,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
@@ -3563,7 +3577,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="1" t="s">
         <v>103</v>
       </c>
@@ -3575,7 +3589,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="1" t="s">
         <v>104</v>
       </c>
@@ -3587,7 +3601,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="1" t="s">
         <v>105</v>
       </c>
@@ -3599,7 +3613,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="1" t="s">
         <v>106</v>
       </c>
@@ -3611,7 +3625,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="1" t="s">
         <v>107</v>
       </c>
@@ -3623,7 +3637,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="1" t="s">
         <v>108</v>
       </c>
@@ -3635,7 +3649,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="16"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="1" t="s">
         <v>109</v>
       </c>
@@ -3647,7 +3661,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="16"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="1" t="s">
         <v>60</v>
       </c>
@@ -3659,7 +3673,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="16"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="1" t="s">
         <v>110</v>
       </c>
@@ -3671,7 +3685,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="16"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="1" t="s">
         <v>111</v>
       </c>
@@ -3683,7 +3697,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
+      <c r="A28" s="38"/>
       <c r="B28" s="1" t="s">
         <v>112</v>
       </c>
@@ -3695,7 +3709,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="37" t="s">
         <v>53</v>
       </c>
       <c r="B29" s="1"/>
@@ -3707,7 +3721,7 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="1" t="s">
         <v>69</v>
       </c>
@@ -3721,7 +3735,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="16"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="1" t="s">
         <v>72</v>
       </c>
@@ -3735,7 +3749,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="16"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="1" t="s">
         <v>118</v>
       </c>
@@ -3749,7 +3763,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="4" t="s">
         <v>120</v>
       </c>
@@ -3763,7 +3777,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="1" t="s">
         <v>84</v>
       </c>
@@ -3777,7 +3791,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="16"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="1" t="s">
         <v>123</v>
       </c>
@@ -3791,7 +3805,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
+      <c r="A36" s="40"/>
       <c r="B36" s="1" t="s">
         <v>125</v>
       </c>
@@ -3805,7 +3819,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="16"/>
+      <c r="A37" s="40"/>
       <c r="B37" s="1" t="s">
         <v>127</v>
       </c>
@@ -3819,7 +3833,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
+      <c r="A38" s="40"/>
       <c r="B38" s="1" t="s">
         <v>129</v>
       </c>
@@ -3833,7 +3847,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="16"/>
+      <c r="A39" s="40"/>
       <c r="B39" s="1" t="s">
         <v>131</v>
       </c>
@@ -3847,7 +3861,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="16"/>
+      <c r="A40" s="40"/>
       <c r="B40" s="1" t="s">
         <v>133</v>
       </c>
@@ -3861,7 +3875,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="16"/>
+      <c r="A41" s="40"/>
       <c r="B41" s="1" t="s">
         <v>135</v>
       </c>
@@ -3875,7 +3889,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="16"/>
+      <c r="A42" s="40"/>
       <c r="B42" s="1" t="s">
         <v>137</v>
       </c>
@@ -3889,7 +3903,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="16"/>
+      <c r="A43" s="40"/>
       <c r="B43" s="1" t="s">
         <v>139</v>
       </c>
@@ -3903,7 +3917,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="16"/>
+      <c r="A44" s="40"/>
       <c r="B44" s="1" t="s">
         <v>141</v>
       </c>
@@ -3917,7 +3931,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="16"/>
+      <c r="A45" s="40"/>
       <c r="B45" s="1" t="s">
         <v>143</v>
       </c>
@@ -3931,7 +3945,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="16"/>
+      <c r="A46" s="40"/>
       <c r="B46" s="1" t="s">
         <v>145</v>
       </c>
@@ -3945,7 +3959,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="16"/>
+      <c r="A47" s="40"/>
       <c r="B47" s="1" t="s">
         <v>147</v>
       </c>
@@ -3959,7 +3973,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="16"/>
+      <c r="A48" s="40"/>
       <c r="B48" s="1" t="s">
         <v>149</v>
       </c>
@@ -3973,7 +3987,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="16"/>
+      <c r="A49" s="40"/>
       <c r="B49" s="1" t="s">
         <v>151</v>
       </c>
@@ -3987,7 +4001,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="16"/>
+      <c r="A50" s="40"/>
       <c r="B50" s="1" t="s">
         <v>153</v>
       </c>
@@ -4001,7 +4015,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="16"/>
+      <c r="A51" s="40"/>
       <c r="B51" s="1" t="s">
         <v>155</v>
       </c>
@@ -4015,7 +4029,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="16"/>
+      <c r="A52" s="40"/>
       <c r="B52" s="1" t="s">
         <v>157</v>
       </c>
@@ -4029,7 +4043,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="16"/>
+      <c r="A53" s="40"/>
       <c r="B53" s="1" t="s">
         <v>159</v>
       </c>
@@ -4043,7 +4057,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="17"/>
+      <c r="A54" s="38"/>
       <c r="B54" s="1" t="s">
         <v>161</v>
       </c>
@@ -4057,7 +4071,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B55" s="1"/>
@@ -4071,7 +4085,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="16"/>
+      <c r="A56" s="40"/>
       <c r="B56" s="1" t="s">
         <v>163</v>
       </c>
@@ -4083,7 +4097,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="16"/>
+      <c r="A57" s="40"/>
       <c r="B57" s="1" t="s">
         <v>164</v>
       </c>
@@ -4099,7 +4113,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="16"/>
+      <c r="A58" s="40"/>
       <c r="B58" s="1" t="s">
         <v>165</v>
       </c>
@@ -4115,7 +4129,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="16"/>
+      <c r="A59" s="40"/>
       <c r="B59" s="1" t="s">
         <v>166</v>
       </c>
@@ -4131,7 +4145,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="17"/>
+      <c r="A60" s="38"/>
       <c r="B60" s="1" t="s">
         <v>167</v>
       </c>
@@ -4143,7 +4157,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="45" t="s">
         <v>5</v>
       </c>
       <c r="B61" s="4"/>
@@ -4157,7 +4171,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="18"/>
+      <c r="A62" s="45"/>
       <c r="B62" s="4" t="s">
         <v>169</v>
       </c>
@@ -4169,7 +4183,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="18"/>
+      <c r="A63" s="45"/>
       <c r="B63" s="4" t="s">
         <v>170</v>
       </c>
@@ -4185,7 +4199,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A64" s="18"/>
+      <c r="A64" s="45"/>
       <c r="B64" s="4" t="s">
         <v>171</v>
       </c>
@@ -4201,7 +4215,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="18"/>
+      <c r="A65" s="45"/>
       <c r="B65" s="4" t="s">
         <v>172</v>
       </c>
@@ -4231,7 +4245,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="41" t="s">
         <v>7</v>
       </c>
       <c r="B67" s="4"/>
@@ -4247,7 +4261,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A68" s="19"/>
+      <c r="A68" s="41"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4" t="s">
         <v>185</v>
@@ -4259,7 +4273,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A69" s="19"/>
+      <c r="A69" s="41"/>
       <c r="B69" s="4" t="s">
         <v>180</v>
       </c>
@@ -4273,7 +4287,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="19"/>
+      <c r="A70" s="41"/>
       <c r="B70" s="4" t="s">
         <v>181</v>
       </c>
@@ -4287,7 +4301,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="19"/>
+      <c r="A71" s="41"/>
       <c r="B71" s="4" t="s">
         <v>182</v>
       </c>
@@ -4301,7 +4315,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="19"/>
+      <c r="A72" s="41"/>
       <c r="B72" s="4" t="s">
         <v>186</v>
       </c>
@@ -4315,7 +4329,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="19"/>
+      <c r="A73" s="41"/>
       <c r="B73" s="4" t="s">
         <v>188</v>
       </c>
@@ -4327,7 +4341,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="19"/>
+      <c r="A74" s="41"/>
       <c r="B74" s="4" t="s">
         <v>189</v>
       </c>
@@ -4343,7 +4357,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A75" s="19"/>
+      <c r="A75" s="41"/>
       <c r="B75" s="4" t="s">
         <v>192</v>
       </c>
@@ -4359,7 +4373,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A76" s="19"/>
+      <c r="A76" s="41"/>
       <c r="B76" s="4" t="s">
         <v>195</v>
       </c>
@@ -4375,7 +4389,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="19"/>
+      <c r="A77" s="41"/>
       <c r="B77" s="4" t="s">
         <v>198</v>
       </c>
@@ -4389,7 +4403,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A78" s="19"/>
+      <c r="A78" s="41"/>
       <c r="B78" s="4" t="s">
         <v>200</v>
       </c>
@@ -4405,7 +4419,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="19"/>
+      <c r="A79" s="41"/>
       <c r="B79" s="4" t="s">
         <v>202</v>
       </c>
@@ -4421,7 +4435,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="19"/>
+      <c r="A80" s="41"/>
       <c r="B80" s="4" t="s">
         <v>205</v>
       </c>
@@ -4437,7 +4451,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A81" s="19"/>
+      <c r="A81" s="41"/>
       <c r="B81" s="4" t="s">
         <v>208</v>
       </c>
@@ -4453,7 +4467,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A82" s="15" t="s">
+      <c r="A82" s="37" t="s">
         <v>44</v>
       </c>
       <c r="B82" s="4"/>
@@ -4469,7 +4483,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="17"/>
+      <c r="A83" s="38"/>
       <c r="B83" s="4" t="s">
         <v>288</v>
       </c>
@@ -4481,7 +4495,7 @@
       <c r="F83" s="7"/>
     </row>
     <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A84" s="22" t="s">
+      <c r="A84" s="36" t="s">
         <v>282</v>
       </c>
       <c r="B84" s="1"/>
@@ -4495,7 +4509,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A85" s="22"/>
+      <c r="A85" s="36"/>
       <c r="B85" s="1"/>
       <c r="C85" s="4" t="s">
         <v>219</v>
@@ -4509,7 +4523,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="22"/>
+      <c r="A86" s="36"/>
       <c r="B86" s="1"/>
       <c r="C86" s="4" t="s">
         <v>229</v>
@@ -4521,7 +4535,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A87" s="22"/>
+      <c r="A87" s="36"/>
       <c r="B87" s="1"/>
       <c r="C87" s="4" t="s">
         <v>279</v>
@@ -4533,7 +4547,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="22"/>
+      <c r="A88" s="36"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
         <v>281</v>
@@ -4545,7 +4559,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="22"/>
+      <c r="A89" s="36"/>
       <c r="B89" s="4" t="s">
         <v>180</v>
       </c>
@@ -4557,7 +4571,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="22"/>
+      <c r="A90" s="36"/>
       <c r="B90" s="4" t="s">
         <v>181</v>
       </c>
@@ -4569,7 +4583,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A91" s="22"/>
+      <c r="A91" s="36"/>
       <c r="B91" s="4" t="s">
         <v>230</v>
       </c>
@@ -4581,7 +4595,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A92" s="22"/>
+      <c r="A92" s="36"/>
       <c r="B92" s="10" t="s">
         <v>218</v>
       </c>
@@ -4595,7 +4609,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="22"/>
+      <c r="A93" s="36"/>
       <c r="B93" s="4" t="s">
         <v>9</v>
       </c>
@@ -4609,7 +4623,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="22"/>
+      <c r="A94" s="36"/>
       <c r="B94" s="4" t="s">
         <v>215</v>
       </c>
@@ -4623,7 +4637,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="22"/>
+      <c r="A95" s="36"/>
       <c r="B95" s="4" t="s">
         <v>216</v>
       </c>
@@ -4635,7 +4649,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="22"/>
+      <c r="A96" s="36"/>
       <c r="B96" s="4" t="s">
         <v>221</v>
       </c>
@@ -4649,7 +4663,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="22"/>
+      <c r="A97" s="36"/>
       <c r="B97" s="4" t="s">
         <v>223</v>
       </c>
@@ -4663,7 +4677,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="22"/>
+      <c r="A98" s="36"/>
       <c r="B98" s="4" t="s">
         <v>225</v>
       </c>
@@ -4677,7 +4691,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="22"/>
+      <c r="A99" s="36"/>
       <c r="B99" s="4" t="s">
         <v>227</v>
       </c>
@@ -4705,7 +4719,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="15" t="s">
+      <c r="A101" s="37" t="s">
         <v>59</v>
       </c>
       <c r="B101" s="4"/>
@@ -4719,7 +4733,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" s="16"/>
+      <c r="A102" s="40"/>
       <c r="B102" s="4" t="s">
         <v>284</v>
       </c>
@@ -4729,7 +4743,7 @@
       <c r="F102" s="7"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" s="16"/>
+      <c r="A103" s="40"/>
       <c r="B103" s="4" t="s">
         <v>285</v>
       </c>
@@ -4739,7 +4753,7 @@
       <c r="F103" s="7"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" s="17"/>
+      <c r="A104" s="38"/>
       <c r="B104" s="4" t="s">
         <v>286</v>
       </c>
@@ -4749,7 +4763,7 @@
       <c r="F104" s="7"/>
     </row>
     <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A105" s="22" t="s">
+      <c r="A105" s="36" t="s">
         <v>10</v>
       </c>
       <c r="B105" s="1"/>
@@ -4765,7 +4779,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" s="22"/>
+      <c r="A106" s="36"/>
       <c r="B106" s="4" t="s">
         <v>232</v>
       </c>
@@ -4779,7 +4793,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107" s="22"/>
+      <c r="A107" s="36"/>
       <c r="B107" s="4" t="s">
         <v>233</v>
       </c>
@@ -4795,7 +4809,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="22" t="s">
+      <c r="A108" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B108" s="1"/>
@@ -4809,7 +4823,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" s="22"/>
+      <c r="A109" s="36"/>
       <c r="B109" s="4" t="s">
         <v>234</v>
       </c>
@@ -4823,7 +4837,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A110" s="22" t="s">
+      <c r="A110" s="36" t="s">
         <v>236</v>
       </c>
       <c r="B110" s="1"/>
@@ -4841,7 +4855,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A111" s="22"/>
+      <c r="A111" s="36"/>
       <c r="B111" s="4" t="s">
         <v>240</v>
       </c>
@@ -4855,7 +4869,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="22"/>
+      <c r="A112" s="36"/>
       <c r="B112" s="1" t="s">
         <v>242</v>
       </c>
@@ -4871,7 +4885,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" s="22"/>
+      <c r="A113" s="36"/>
       <c r="B113" s="4" t="s">
         <v>244</v>
       </c>
@@ -4887,7 +4901,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A114" s="22"/>
+      <c r="A114" s="36"/>
       <c r="B114" s="1" t="s">
         <v>245</v>
       </c>
@@ -4905,7 +4919,7 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" s="22"/>
+      <c r="A115" s="36"/>
       <c r="B115" s="4" t="s">
         <v>247</v>
       </c>
@@ -4919,7 +4933,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A116" s="22" t="s">
+      <c r="A116" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B116" s="1"/>
@@ -4933,7 +4947,7 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="22"/>
+      <c r="A117" s="36"/>
       <c r="B117" s="4" t="s">
         <v>250</v>
       </c>
@@ -4945,7 +4959,7 @@
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="22" t="s">
+      <c r="A118" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B118" s="1"/>
@@ -4959,7 +4973,7 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="22"/>
+      <c r="A119" s="36"/>
       <c r="B119" s="4" t="s">
         <v>252</v>
       </c>
@@ -4971,7 +4985,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="22"/>
+      <c r="A120" s="36"/>
       <c r="B120" s="1" t="s">
         <v>253</v>
       </c>
@@ -4983,7 +4997,7 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="22"/>
+      <c r="A121" s="36"/>
       <c r="B121" s="4" t="s">
         <v>254</v>
       </c>
@@ -4997,7 +5011,7 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122" s="22"/>
+      <c r="A122" s="36"/>
       <c r="B122" s="1" t="s">
         <v>256</v>
       </c>
@@ -5011,7 +5025,7 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123" s="22" t="s">
+      <c r="A123" s="36" t="s">
         <v>15</v>
       </c>
       <c r="B123" s="1"/>
@@ -5025,7 +5039,7 @@
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" s="22"/>
+      <c r="A124" s="36"/>
       <c r="B124" s="1" t="s">
         <v>259</v>
       </c>
@@ -5037,7 +5051,7 @@
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A125" s="22"/>
+      <c r="A125" s="36"/>
       <c r="B125" s="1" t="s">
         <v>253</v>
       </c>
@@ -5051,7 +5065,7 @@
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A126" s="22"/>
+      <c r="A126" s="36"/>
       <c r="B126" s="1" t="s">
         <v>254</v>
       </c>
@@ -5065,7 +5079,7 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127" s="22"/>
+      <c r="A127" s="36"/>
       <c r="B127" s="1" t="s">
         <v>256</v>
       </c>
@@ -5079,7 +5093,7 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" s="22"/>
+      <c r="A128" s="36"/>
       <c r="B128" s="1" t="s">
         <v>263</v>
       </c>
@@ -5093,7 +5107,7 @@
       </c>
     </row>
     <row r="129" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="15" t="s">
+      <c r="A129" s="37" t="s">
         <v>16</v>
       </c>
       <c r="B129" s="1"/>
@@ -5109,7 +5123,7 @@
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A130" s="16"/>
+      <c r="A130" s="40"/>
       <c r="B130" s="1" t="s">
         <v>267</v>
       </c>
@@ -5123,7 +5137,7 @@
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A131" s="16"/>
+      <c r="A131" s="40"/>
       <c r="B131" s="1" t="s">
         <v>269</v>
       </c>
@@ -5135,7 +5149,7 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" s="16"/>
+      <c r="A132" s="40"/>
       <c r="B132" s="1" t="s">
         <v>125</v>
       </c>
@@ -5147,7 +5161,7 @@
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A133" s="16"/>
+      <c r="A133" s="40"/>
       <c r="B133" s="1" t="s">
         <v>270</v>
       </c>
@@ -5159,7 +5173,7 @@
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A134" s="16"/>
+      <c r="A134" s="40"/>
       <c r="B134" s="1" t="s">
         <v>271</v>
       </c>
@@ -5171,7 +5185,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A135" s="16"/>
+      <c r="A135" s="40"/>
       <c r="B135" s="1" t="s">
         <v>272</v>
       </c>
@@ -5183,7 +5197,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A136" s="16"/>
+      <c r="A136" s="40"/>
       <c r="B136" s="1" t="s">
         <v>273</v>
       </c>
@@ -5195,7 +5209,7 @@
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A137" s="16"/>
+      <c r="A137" s="40"/>
       <c r="B137" s="1" t="s">
         <v>274</v>
       </c>
@@ -5207,7 +5221,7 @@
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A138" s="16"/>
+      <c r="A138" s="40"/>
       <c r="B138" s="1" t="s">
         <v>275</v>
       </c>
@@ -5219,7 +5233,7 @@
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A139" s="17"/>
+      <c r="A139" s="38"/>
       <c r="B139" s="1" t="s">
         <v>276</v>
       </c>
@@ -5231,7 +5245,7 @@
       </c>
     </row>
     <row r="140" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="20" t="s">
+      <c r="A140" s="46" t="s">
         <v>17</v>
       </c>
       <c r="B140" s="1"/>
@@ -5245,7 +5259,7 @@
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A141" s="21"/>
+      <c r="A141" s="44"/>
       <c r="B141" s="1" t="s">
         <v>278</v>
       </c>
@@ -5257,7 +5271,7 @@
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A142" s="15" t="s">
+      <c r="A142" s="37" t="s">
         <v>27</v>
       </c>
       <c r="B142" s="1"/>
@@ -5271,7 +5285,7 @@
       </c>
     </row>
     <row r="143" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A143" s="16"/>
+      <c r="A143" s="40"/>
       <c r="B143" s="4" t="s">
         <v>20</v>
       </c>
@@ -5283,7 +5297,7 @@
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A144" s="16"/>
+      <c r="A144" s="40"/>
       <c r="B144" s="1" t="s">
         <v>21</v>
       </c>
@@ -5295,7 +5309,7 @@
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A145" s="16"/>
+      <c r="A145" s="40"/>
       <c r="B145" s="1" t="s">
         <v>22</v>
       </c>
@@ -5307,7 +5321,7 @@
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A146" s="16"/>
+      <c r="A146" s="40"/>
       <c r="B146" s="1" t="s">
         <v>23</v>
       </c>
@@ -5319,7 +5333,7 @@
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A147" s="16"/>
+      <c r="A147" s="40"/>
       <c r="B147" s="1" t="s">
         <v>24</v>
       </c>
@@ -5331,7 +5345,7 @@
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A148" s="16"/>
+      <c r="A148" s="40"/>
       <c r="B148" s="1" t="s">
         <v>25</v>
       </c>
@@ -5343,7 +5357,7 @@
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A149" s="16"/>
+      <c r="A149" s="40"/>
       <c r="B149" s="1" t="s">
         <v>26</v>
       </c>
@@ -5355,7 +5369,7 @@
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A150" s="16"/>
+      <c r="A150" s="40"/>
       <c r="B150" s="1" t="s">
         <v>32</v>
       </c>
@@ -5367,7 +5381,7 @@
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A151" s="16"/>
+      <c r="A151" s="40"/>
       <c r="B151" s="1" t="s">
         <v>33</v>
       </c>
@@ -5379,7 +5393,7 @@
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A152" s="16"/>
+      <c r="A152" s="40"/>
       <c r="B152" s="1" t="s">
         <v>35</v>
       </c>
@@ -5391,7 +5405,7 @@
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A153" s="16"/>
+      <c r="A153" s="40"/>
       <c r="B153" s="1" t="s">
         <v>36</v>
       </c>
@@ -5403,7 +5417,7 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A154" s="17"/>
+      <c r="A154" s="38"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
@@ -5413,7 +5427,7 @@
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A155" s="15" t="s">
+      <c r="A155" s="37" t="s">
         <v>29</v>
       </c>
       <c r="B155" s="1"/>
@@ -5427,7 +5441,7 @@
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A156" s="16"/>
+      <c r="A156" s="40"/>
       <c r="B156" s="1" t="s">
         <v>30</v>
       </c>
@@ -5439,7 +5453,7 @@
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A157" s="16"/>
+      <c r="A157" s="40"/>
       <c r="B157" s="1" t="s">
         <v>37</v>
       </c>
@@ -5451,7 +5465,7 @@
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A158" s="16"/>
+      <c r="A158" s="40"/>
       <c r="B158" s="1" t="s">
         <v>40</v>
       </c>
@@ -5463,7 +5477,7 @@
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A159" s="16"/>
+      <c r="A159" s="40"/>
       <c r="B159" s="1" t="s">
         <v>41</v>
       </c>
@@ -5477,7 +5491,7 @@
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A160" s="16"/>
+      <c r="A160" s="40"/>
       <c r="B160" s="1" t="s">
         <v>39</v>
       </c>
@@ -5491,7 +5505,7 @@
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A161" s="17"/>
+      <c r="A161" s="38"/>
       <c r="B161" s="1" t="s">
         <v>43</v>
       </c>
@@ -5503,7 +5517,7 @@
       </c>
     </row>
     <row r="162" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A162" s="15" t="s">
+      <c r="A162" s="37" t="s">
         <v>45</v>
       </c>
       <c r="B162" s="1"/>
@@ -5521,7 +5535,7 @@
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A163" s="17"/>
+      <c r="A163" s="38"/>
       <c r="B163" s="1" t="s">
         <v>346</v>
       </c>
@@ -5533,7 +5547,7 @@
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A164" s="24" t="s">
+      <c r="A164" s="42" t="s">
         <v>347</v>
       </c>
       <c r="B164" s="8" t="s">
@@ -5553,7 +5567,7 @@
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A165" s="25"/>
+      <c r="A165" s="43"/>
       <c r="B165" s="8" t="s">
         <v>47</v>
       </c>
@@ -5571,7 +5585,7 @@
       </c>
     </row>
     <row r="166" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A166" s="25"/>
+      <c r="A166" s="43"/>
       <c r="B166" s="8" t="s">
         <v>297</v>
       </c>
@@ -5589,7 +5603,7 @@
       </c>
     </row>
     <row r="167" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A167" s="21"/>
+      <c r="A167" s="44"/>
       <c r="B167" s="8" t="s">
         <v>49</v>
       </c>
@@ -5679,7 +5693,7 @@
       </c>
     </row>
     <row r="173" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A173" s="15" t="s">
+      <c r="A173" s="37" t="s">
         <v>312</v>
       </c>
       <c r="B173" s="1"/>
@@ -5693,7 +5707,7 @@
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A174" s="16"/>
+      <c r="A174" s="40"/>
       <c r="B174" s="1" t="s">
         <v>284</v>
       </c>
@@ -5705,7 +5719,7 @@
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A175" s="16"/>
+      <c r="A175" s="40"/>
       <c r="B175" s="1" t="s">
         <v>285</v>
       </c>
@@ -5717,7 +5731,7 @@
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A176" s="16"/>
+      <c r="A176" s="40"/>
       <c r="B176" s="1" t="s">
         <v>253</v>
       </c>
@@ -5729,7 +5743,7 @@
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A177" s="16"/>
+      <c r="A177" s="40"/>
       <c r="B177" s="1" t="s">
         <v>314</v>
       </c>
@@ -5741,7 +5755,7 @@
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A178" s="17"/>
+      <c r="A178" s="38"/>
       <c r="B178" s="1" t="s">
         <v>315</v>
       </c>
@@ -5753,7 +5767,7 @@
       </c>
     </row>
     <row r="179" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A179" s="19" t="s">
+      <c r="A179" s="41" t="s">
         <v>6</v>
       </c>
       <c r="B179" s="4"/>
@@ -5767,7 +5781,7 @@
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A180" s="19"/>
+      <c r="A180" s="41"/>
       <c r="B180" s="4" t="s">
         <v>69</v>
       </c>
@@ -5779,7 +5793,7 @@
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A181" s="19"/>
+      <c r="A181" s="41"/>
       <c r="B181" s="4" t="s">
         <v>72</v>
       </c>
@@ -5791,7 +5805,7 @@
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A182" s="19"/>
+      <c r="A182" s="41"/>
       <c r="B182" s="4" t="s">
         <v>176</v>
       </c>
@@ -5803,7 +5817,7 @@
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A183" s="19"/>
+      <c r="A183" s="41"/>
       <c r="B183" s="4" t="s">
         <v>177</v>
       </c>
@@ -5815,7 +5829,7 @@
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A184" s="19"/>
+      <c r="A184" s="41"/>
       <c r="B184" s="4" t="s">
         <v>178</v>
       </c>
@@ -5827,7 +5841,7 @@
       </c>
     </row>
     <row r="185" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A185" s="15" t="s">
+      <c r="A185" s="37" t="s">
         <v>60</v>
       </c>
       <c r="B185" s="1"/>
@@ -5841,7 +5855,7 @@
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A186" s="16"/>
+      <c r="A186" s="40"/>
       <c r="B186" s="7" t="s">
         <v>60</v>
       </c>
@@ -5855,7 +5869,7 @@
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A187" s="16"/>
+      <c r="A187" s="40"/>
       <c r="B187" s="7" t="s">
         <v>319</v>
       </c>
@@ -5869,7 +5883,7 @@
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A188" s="16"/>
+      <c r="A188" s="40"/>
       <c r="B188" s="7" t="s">
         <v>285</v>
       </c>
@@ -5883,7 +5897,7 @@
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A189" s="16"/>
+      <c r="A189" s="40"/>
       <c r="B189" s="7" t="s">
         <v>322</v>
       </c>
@@ -5897,7 +5911,7 @@
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A190" s="16"/>
+      <c r="A190" s="40"/>
       <c r="B190" s="7" t="s">
         <v>324</v>
       </c>
@@ -5911,7 +5925,7 @@
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A191" s="16"/>
+      <c r="A191" s="40"/>
       <c r="B191" s="7" t="s">
         <v>326</v>
       </c>
@@ -5925,7 +5939,7 @@
       </c>
     </row>
     <row r="192" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A192" s="16"/>
+      <c r="A192" s="40"/>
       <c r="B192" s="7" t="s">
         <v>328</v>
       </c>
@@ -5939,7 +5953,7 @@
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A193" s="16"/>
+      <c r="A193" s="40"/>
       <c r="B193" s="7" t="s">
         <v>330</v>
       </c>
@@ -5953,7 +5967,7 @@
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A194" s="16"/>
+      <c r="A194" s="40"/>
       <c r="B194" s="7" t="s">
         <v>332</v>
       </c>
@@ -5967,7 +5981,7 @@
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A195" s="17"/>
+      <c r="A195" s="38"/>
       <c r="B195" s="7" t="s">
         <v>334</v>
       </c>
@@ -5981,7 +5995,7 @@
       </c>
     </row>
     <row r="196" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A196" s="15" t="s">
+      <c r="A196" s="37" t="s">
         <v>61</v>
       </c>
       <c r="B196" s="1"/>
@@ -5995,7 +6009,7 @@
       </c>
     </row>
     <row r="197" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A197" s="16"/>
+      <c r="A197" s="40"/>
       <c r="B197" s="7" t="s">
         <v>60</v>
       </c>
@@ -6009,7 +6023,7 @@
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A198" s="16"/>
+      <c r="A198" s="40"/>
       <c r="B198" s="7" t="s">
         <v>61</v>
       </c>
@@ -6023,7 +6037,7 @@
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A199" s="16"/>
+      <c r="A199" s="40"/>
       <c r="B199" s="7" t="s">
         <v>285</v>
       </c>
@@ -6037,7 +6051,7 @@
       </c>
     </row>
     <row r="200" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A200" s="16"/>
+      <c r="A200" s="40"/>
       <c r="B200" s="7" t="s">
         <v>328</v>
       </c>
@@ -6051,7 +6065,7 @@
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A201" s="16"/>
+      <c r="A201" s="40"/>
       <c r="B201" s="7" t="s">
         <v>341</v>
       </c>
@@ -6065,7 +6079,7 @@
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A202" s="16"/>
+      <c r="A202" s="40"/>
       <c r="B202" s="7" t="s">
         <v>343</v>
       </c>
@@ -6079,7 +6093,7 @@
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A203" s="16"/>
+      <c r="A203" s="40"/>
       <c r="B203" s="7" t="s">
         <v>348</v>
       </c>
@@ -6093,7 +6107,7 @@
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A204" s="16"/>
+      <c r="A204" s="40"/>
       <c r="B204" s="7" t="s">
         <v>350</v>
       </c>
@@ -6107,7 +6121,7 @@
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A205" s="16"/>
+      <c r="A205" s="40"/>
       <c r="B205" s="7" t="s">
         <v>352</v>
       </c>
@@ -6121,7 +6135,7 @@
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A206" s="17"/>
+      <c r="A206" s="38"/>
       <c r="B206" s="7" t="s">
         <v>111</v>
       </c>
@@ -6135,7 +6149,7 @@
       </c>
     </row>
     <row r="207" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A207" s="22" t="s">
+      <c r="A207" s="36" t="s">
         <v>62</v>
       </c>
       <c r="B207" s="1"/>
@@ -6149,7 +6163,7 @@
       </c>
     </row>
     <row r="208" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A208" s="22"/>
+      <c r="A208" s="36"/>
       <c r="B208" s="7" t="s">
         <v>60</v>
       </c>
@@ -6163,7 +6177,7 @@
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A209" s="22"/>
+      <c r="A209" s="36"/>
       <c r="B209" s="7" t="s">
         <v>61</v>
       </c>
@@ -6177,7 +6191,7 @@
       </c>
     </row>
     <row r="210" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A210" s="22"/>
+      <c r="A210" s="36"/>
       <c r="B210" s="7" t="s">
         <v>359</v>
       </c>
@@ -6191,7 +6205,7 @@
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A211" s="22"/>
+      <c r="A211" s="36"/>
       <c r="B211" s="7" t="s">
         <v>361</v>
       </c>
@@ -6205,7 +6219,7 @@
       </c>
     </row>
     <row r="212" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A212" s="22"/>
+      <c r="A212" s="36"/>
       <c r="B212" s="7" t="s">
         <v>363</v>
       </c>
@@ -6219,7 +6233,7 @@
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A213" s="22"/>
+      <c r="A213" s="36"/>
       <c r="B213" s="7" t="s">
         <v>365</v>
       </c>
@@ -6233,7 +6247,7 @@
       </c>
     </row>
     <row r="214" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A214" s="22"/>
+      <c r="A214" s="36"/>
       <c r="B214" s="7" t="s">
         <v>367</v>
       </c>
@@ -6247,7 +6261,7 @@
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A215" s="22"/>
+      <c r="A215" s="36"/>
       <c r="B215" s="7" t="s">
         <v>369</v>
       </c>
@@ -6261,7 +6275,7 @@
       </c>
     </row>
     <row r="216" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A216" s="22"/>
+      <c r="A216" s="36"/>
       <c r="B216" s="7" t="s">
         <v>371</v>
       </c>
@@ -6275,7 +6289,7 @@
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A217" s="22"/>
+      <c r="A217" s="36"/>
       <c r="B217" s="7" t="s">
         <v>373</v>
       </c>
@@ -6289,7 +6303,7 @@
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A218" s="22"/>
+      <c r="A218" s="36"/>
       <c r="B218" s="7" t="s">
         <v>375</v>
       </c>
@@ -6303,7 +6317,7 @@
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A219" s="22"/>
+      <c r="A219" s="36"/>
       <c r="B219" s="7" t="s">
         <v>377</v>
       </c>
@@ -6317,7 +6331,7 @@
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A220" s="22"/>
+      <c r="A220" s="36"/>
       <c r="B220" s="7" t="s">
         <v>379</v>
       </c>
@@ -6331,7 +6345,7 @@
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A221" s="22"/>
+      <c r="A221" s="36"/>
       <c r="B221" s="7" t="s">
         <v>381</v>
       </c>
@@ -6345,7 +6359,7 @@
       </c>
     </row>
     <row r="222" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A222" s="22"/>
+      <c r="A222" s="36"/>
       <c r="B222" s="7" t="s">
         <v>383</v>
       </c>
@@ -6359,7 +6373,7 @@
       </c>
     </row>
     <row r="223" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A223" s="22"/>
+      <c r="A223" s="36"/>
       <c r="B223" s="7" t="s">
         <v>385</v>
       </c>
@@ -6373,7 +6387,7 @@
       </c>
     </row>
     <row r="224" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A224" s="22"/>
+      <c r="A224" s="36"/>
       <c r="B224" s="7" t="s">
         <v>387</v>
       </c>
@@ -6387,7 +6401,7 @@
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A225" s="22"/>
+      <c r="A225" s="36"/>
       <c r="B225" s="7" t="s">
         <v>389</v>
       </c>
@@ -6401,7 +6415,7 @@
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A226" s="22"/>
+      <c r="A226" s="36"/>
       <c r="B226" s="7" t="s">
         <v>111</v>
       </c>
@@ -6415,7 +6429,7 @@
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A227" s="22"/>
+      <c r="A227" s="36"/>
       <c r="B227" s="7" t="s">
         <v>392</v>
       </c>
@@ -6429,7 +6443,7 @@
       </c>
     </row>
     <row r="228" spans="1:6" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="22" t="s">
+      <c r="A228" s="36" t="s">
         <v>63</v>
       </c>
       <c r="B228" s="1"/>
@@ -6443,7 +6457,7 @@
       </c>
     </row>
     <row r="229" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A229" s="22"/>
+      <c r="A229" s="36"/>
       <c r="B229" s="7" t="s">
         <v>60</v>
       </c>
@@ -6457,7 +6471,7 @@
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A230" s="22"/>
+      <c r="A230" s="36"/>
       <c r="B230" s="7" t="s">
         <v>61</v>
       </c>
@@ -6471,7 +6485,7 @@
       </c>
     </row>
     <row r="231" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A231" s="22"/>
+      <c r="A231" s="36"/>
       <c r="B231" s="7" t="s">
         <v>359</v>
       </c>
@@ -6485,7 +6499,7 @@
       </c>
     </row>
     <row r="232" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A232" s="22"/>
+      <c r="A232" s="36"/>
       <c r="B232" s="7" t="s">
         <v>361</v>
       </c>
@@ -6499,7 +6513,7 @@
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A233" s="22"/>
+      <c r="A233" s="36"/>
       <c r="B233" s="7" t="s">
         <v>398</v>
       </c>
@@ -6513,7 +6527,7 @@
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A234" s="22"/>
+      <c r="A234" s="36"/>
       <c r="B234" s="7" t="s">
         <v>400</v>
       </c>
@@ -6527,7 +6541,7 @@
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A235" s="22"/>
+      <c r="A235" s="36"/>
       <c r="B235" s="7" t="s">
         <v>402</v>
       </c>
@@ -6541,7 +6555,7 @@
       </c>
     </row>
     <row r="236" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A236" s="22"/>
+      <c r="A236" s="36"/>
       <c r="B236" s="7" t="s">
         <v>365</v>
       </c>
@@ -6555,7 +6569,7 @@
       </c>
     </row>
     <row r="237" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A237" s="22"/>
+      <c r="A237" s="36"/>
       <c r="B237" s="7" t="s">
         <v>367</v>
       </c>
@@ -6569,7 +6583,7 @@
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A238" s="22"/>
+      <c r="A238" s="36"/>
       <c r="B238" s="7" t="s">
         <v>406</v>
       </c>
@@ -6583,7 +6597,7 @@
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A239" s="22"/>
+      <c r="A239" s="36"/>
       <c r="B239" s="7" t="s">
         <v>373</v>
       </c>
@@ -6597,7 +6611,7 @@
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A240" s="22"/>
+      <c r="A240" s="36"/>
       <c r="B240" s="7" t="s">
         <v>375</v>
       </c>
@@ -6611,7 +6625,7 @@
       </c>
     </row>
     <row r="241" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A241" s="22"/>
+      <c r="A241" s="36"/>
       <c r="B241" s="7" t="s">
         <v>410</v>
       </c>
@@ -6625,7 +6639,7 @@
       </c>
     </row>
     <row r="242" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A242" s="22"/>
+      <c r="A242" s="36"/>
       <c r="B242" s="7" t="s">
         <v>412</v>
       </c>
@@ -6639,7 +6653,7 @@
       </c>
     </row>
     <row r="243" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A243" s="22"/>
+      <c r="A243" s="36"/>
       <c r="B243" s="7" t="s">
         <v>414</v>
       </c>
@@ -6653,7 +6667,7 @@
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A244" s="22"/>
+      <c r="A244" s="36"/>
       <c r="B244" s="7" t="s">
         <v>389</v>
       </c>
@@ -6667,7 +6681,7 @@
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A245" s="22"/>
+      <c r="A245" s="36"/>
       <c r="B245" s="7" t="s">
         <v>111</v>
       </c>
@@ -6681,7 +6695,7 @@
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A246" s="22"/>
+      <c r="A246" s="36"/>
       <c r="B246" s="7" t="s">
         <v>392</v>
       </c>
@@ -6695,7 +6709,7 @@
       </c>
     </row>
     <row r="247" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A247" s="23" t="s">
+      <c r="A247" s="39" t="s">
         <v>64</v>
       </c>
       <c r="B247" s="1"/>
@@ -6709,7 +6723,7 @@
       </c>
     </row>
     <row r="248" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A248" s="23"/>
+      <c r="A248" s="39"/>
       <c r="B248" s="7" t="s">
         <v>60</v>
       </c>
@@ -6723,7 +6737,7 @@
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A249" s="23"/>
+      <c r="A249" s="39"/>
       <c r="B249" s="7" t="s">
         <v>61</v>
       </c>
@@ -6737,7 +6751,7 @@
       </c>
     </row>
     <row r="250" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A250" s="23"/>
+      <c r="A250" s="39"/>
       <c r="B250" s="7" t="s">
         <v>359</v>
       </c>
@@ -6751,7 +6765,7 @@
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A251" s="23"/>
+      <c r="A251" s="39"/>
       <c r="B251" s="7" t="s">
         <v>361</v>
       </c>
@@ -6765,7 +6779,7 @@
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A252" s="23"/>
+      <c r="A252" s="39"/>
       <c r="B252" s="7" t="s">
         <v>398</v>
       </c>
@@ -6779,7 +6793,7 @@
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A253" s="23"/>
+      <c r="A253" s="39"/>
       <c r="B253" s="7" t="s">
         <v>425</v>
       </c>
@@ -6793,7 +6807,7 @@
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A254" s="23"/>
+      <c r="A254" s="39"/>
       <c r="B254" s="7" t="s">
         <v>427</v>
       </c>
@@ -6807,7 +6821,7 @@
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A255" s="23"/>
+      <c r="A255" s="39"/>
       <c r="B255" s="7" t="s">
         <v>365</v>
       </c>
@@ -6821,7 +6835,7 @@
       </c>
     </row>
     <row r="256" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A256" s="23"/>
+      <c r="A256" s="39"/>
       <c r="B256" s="7" t="s">
         <v>430</v>
       </c>
@@ -6835,7 +6849,7 @@
       </c>
     </row>
     <row r="257" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A257" s="23"/>
+      <c r="A257" s="39"/>
       <c r="B257" s="7" t="s">
         <v>432</v>
       </c>
@@ -6849,7 +6863,7 @@
       </c>
     </row>
     <row r="258" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A258" s="22" t="s">
+      <c r="A258" s="36" t="s">
         <v>65</v>
       </c>
       <c r="B258" s="1"/>
@@ -6863,7 +6877,7 @@
       </c>
     </row>
     <row r="259" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A259" s="22"/>
+      <c r="A259" s="36"/>
       <c r="B259" s="7" t="s">
         <v>60</v>
       </c>
@@ -6877,7 +6891,7 @@
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A260" s="22"/>
+      <c r="A260" s="36"/>
       <c r="B260" s="7" t="s">
         <v>61</v>
       </c>
@@ -6891,7 +6905,7 @@
       </c>
     </row>
     <row r="261" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A261" s="22"/>
+      <c r="A261" s="36"/>
       <c r="B261" s="7" t="s">
         <v>359</v>
       </c>
@@ -6905,7 +6919,7 @@
       </c>
     </row>
     <row r="262" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A262" s="22"/>
+      <c r="A262" s="36"/>
       <c r="B262" s="7" t="s">
         <v>361</v>
       </c>
@@ -6919,7 +6933,7 @@
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A263" s="22"/>
+      <c r="A263" s="36"/>
       <c r="B263" s="7" t="s">
         <v>398</v>
       </c>
@@ -6933,7 +6947,7 @@
       </c>
     </row>
     <row r="264" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A264" s="22"/>
+      <c r="A264" s="36"/>
       <c r="B264" s="7" t="s">
         <v>440</v>
       </c>
@@ -6947,7 +6961,7 @@
       </c>
     </row>
     <row r="265" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A265" s="22"/>
+      <c r="A265" s="36"/>
       <c r="B265" s="7" t="s">
         <v>442</v>
       </c>
@@ -6961,7 +6975,7 @@
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A266" s="22"/>
+      <c r="A266" s="36"/>
       <c r="B266" s="7" t="s">
         <v>365</v>
       </c>
@@ -6975,7 +6989,7 @@
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A267" s="22"/>
+      <c r="A267" s="36"/>
       <c r="B267" s="7" t="s">
         <v>367</v>
       </c>
@@ -6989,7 +7003,7 @@
       </c>
     </row>
     <row r="268" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A268" s="22"/>
+      <c r="A268" s="36"/>
       <c r="B268" s="7" t="s">
         <v>373</v>
       </c>
@@ -7003,7 +7017,7 @@
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A269" s="22"/>
+      <c r="A269" s="36"/>
       <c r="B269" s="7" t="s">
         <v>447</v>
       </c>
@@ -7017,7 +7031,7 @@
       </c>
     </row>
     <row r="270" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A270" s="22"/>
+      <c r="A270" s="36"/>
       <c r="B270" s="7" t="s">
         <v>449</v>
       </c>
@@ -7031,7 +7045,7 @@
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A271" s="22"/>
+      <c r="A271" s="36"/>
       <c r="B271" s="7" t="s">
         <v>451</v>
       </c>
@@ -7045,7 +7059,7 @@
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A272" s="22"/>
+      <c r="A272" s="36"/>
       <c r="B272" s="7" t="s">
         <v>453</v>
       </c>
@@ -7059,7 +7073,7 @@
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A273" s="22"/>
+      <c r="A273" s="36"/>
       <c r="B273" s="7" t="s">
         <v>389</v>
       </c>
@@ -7073,7 +7087,7 @@
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A274" s="22"/>
+      <c r="A274" s="36"/>
       <c r="B274" s="7" t="s">
         <v>455</v>
       </c>
@@ -7087,7 +7101,7 @@
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A275" s="22"/>
+      <c r="A275" s="36"/>
       <c r="B275" s="7" t="s">
         <v>111</v>
       </c>
@@ -7101,7 +7115,7 @@
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A276" s="22"/>
+      <c r="A276" s="36"/>
       <c r="B276" s="7" t="s">
         <v>392</v>
       </c>
@@ -7115,7 +7129,7 @@
       </c>
     </row>
     <row r="277" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A277" s="22" t="s">
+      <c r="A277" s="36" t="s">
         <v>66</v>
       </c>
       <c r="B277" s="1"/>
@@ -7129,7 +7143,7 @@
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A278" s="22"/>
+      <c r="A278" s="36"/>
       <c r="B278" s="7" t="s">
         <v>60</v>
       </c>
@@ -7143,7 +7157,7 @@
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A279" s="22"/>
+      <c r="A279" s="36"/>
       <c r="B279" s="7" t="s">
         <v>61</v>
       </c>
@@ -7157,7 +7171,7 @@
       </c>
     </row>
     <row r="280" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A280" s="22"/>
+      <c r="A280" s="36"/>
       <c r="B280" s="7" t="s">
         <v>359</v>
       </c>
@@ -7171,7 +7185,7 @@
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A281" s="22"/>
+      <c r="A281" s="36"/>
       <c r="B281" s="7" t="s">
         <v>410</v>
       </c>
@@ -7185,7 +7199,7 @@
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A282" s="22"/>
+      <c r="A282" s="36"/>
       <c r="B282" s="7" t="s">
         <v>464</v>
       </c>
@@ -7199,7 +7213,7 @@
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A283" s="22"/>
+      <c r="A283" s="36"/>
       <c r="B283" s="7" t="s">
         <v>466</v>
       </c>
@@ -7213,7 +7227,7 @@
       </c>
     </row>
     <row r="284" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A284" s="22"/>
+      <c r="A284" s="36"/>
       <c r="B284" s="7" t="s">
         <v>365</v>
       </c>
@@ -7227,7 +7241,7 @@
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A285" s="22"/>
+      <c r="A285" s="36"/>
       <c r="B285" s="7" t="s">
         <v>367</v>
       </c>
@@ -7241,7 +7255,7 @@
       </c>
     </row>
     <row r="286" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A286" s="22"/>
+      <c r="A286" s="36"/>
       <c r="B286" s="7" t="s">
         <v>373</v>
       </c>
@@ -7255,7 +7269,7 @@
       </c>
     </row>
     <row r="287" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A287" s="22"/>
+      <c r="A287" s="36"/>
       <c r="B287" s="7" t="s">
         <v>471</v>
       </c>
@@ -7269,7 +7283,7 @@
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A288" s="22"/>
+      <c r="A288" s="36"/>
       <c r="B288" s="7" t="s">
         <v>473</v>
       </c>
@@ -7283,7 +7297,7 @@
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A289" s="22"/>
+      <c r="A289" s="36"/>
       <c r="B289" s="7" t="s">
         <v>475</v>
       </c>
@@ -7297,7 +7311,7 @@
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A290" s="22"/>
+      <c r="A290" s="36"/>
       <c r="B290" s="7" t="s">
         <v>477</v>
       </c>
@@ -7311,7 +7325,7 @@
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A291" s="22"/>
+      <c r="A291" s="36"/>
       <c r="B291" s="7" t="s">
         <v>479</v>
       </c>
@@ -7325,7 +7339,7 @@
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A292" s="22"/>
+      <c r="A292" s="36"/>
       <c r="B292" s="7" t="s">
         <v>481</v>
       </c>
@@ -7340,19 +7354,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A258:A276"/>
-    <mergeCell ref="A277:A292"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A207:A227"/>
-    <mergeCell ref="A228:A246"/>
-    <mergeCell ref="A247:A257"/>
-    <mergeCell ref="A185:A195"/>
-    <mergeCell ref="A196:A206"/>
-    <mergeCell ref="A173:A178"/>
-    <mergeCell ref="A179:A184"/>
-    <mergeCell ref="A162:A163"/>
-    <mergeCell ref="A164:A167"/>
     <mergeCell ref="A2:A28"/>
     <mergeCell ref="A29:A54"/>
     <mergeCell ref="A55:A60"/>
@@ -7369,6 +7370,19 @@
     <mergeCell ref="A105:A107"/>
     <mergeCell ref="A108:A109"/>
     <mergeCell ref="A110:A115"/>
+    <mergeCell ref="A258:A276"/>
+    <mergeCell ref="A277:A292"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A207:A227"/>
+    <mergeCell ref="A228:A246"/>
+    <mergeCell ref="A247:A257"/>
+    <mergeCell ref="A185:A195"/>
+    <mergeCell ref="A196:A206"/>
+    <mergeCell ref="A173:A178"/>
+    <mergeCell ref="A179:A184"/>
+    <mergeCell ref="A162:A163"/>
+    <mergeCell ref="A164:A167"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates explanatory drawings for linear referencing along Boreholes
</commit_message>
<xml_diff>
--- a/Vocabulary/BoreholeIE_consolidated_vocab.xlsx
+++ b/Vocabulary/BoreholeIE_consolidated_vocab.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040" tabRatio="587" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Spreadsheet_Metadata" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="542">
   <si>
     <t>Concept</t>
   </si>
@@ -1597,9 +1597,6 @@
     <t>color</t>
   </si>
   <si>
-    <t>light orange</t>
-  </si>
-  <si>
     <t xml:space="preserve">BhML rev:6 (EPOS) rationale on logs is the following so far:
 - GeologyLog / LogResult / LogResultElement for discrete logs (where we can identify intervals) building on GWML2 (logical model)
 - for continuous observations or 'outOfBand' situations (large, binary files) the idea is to have an 'OutOfBandResult' type of result </t>
@@ -1671,9 +1668,6 @@
     <t>20190401-1400</t>
   </si>
   <si>
-    <t>light green</t>
-  </si>
-  <si>
     <t>outerRim of BhML, more a reuse of standardized description of Borehole Logs -&gt; out of BhML scope https://github.com/opengeospatial/boreholeie/issues/32</t>
   </si>
   <si>
@@ -1687,6 +1681,18 @@
   </si>
   <si>
     <t>Encoding/Serialization issue not modelling</t>
+  </si>
+  <si>
+    <t>20190415-1400</t>
+  </si>
+  <si>
+    <t>color code removed</t>
+  </si>
+  <si>
+    <t>bold in light blue</t>
+  </si>
+  <si>
+    <t>bold in light green</t>
   </si>
 </sst>
 </file>
@@ -1751,13 +1757,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1827,7 +1833,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1867,18 +1873,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1890,43 +1886,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1935,42 +1898,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2254,19 +2266,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>507</v>
       </c>
@@ -2274,30 +2287,37 @@
         <v>509</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>508</v>
       </c>
       <c r="B2" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="C2" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>532</v>
+      </c>
+      <c r="D2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>510</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>534</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>511</v>
+        <v>540</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>541</v>
+      </c>
+      <c r="D3" t="s">
+        <v>539</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2306,8 +2326,8 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2318,81 +2338,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="25">
+      <c r="C1" s="21">
         <v>2</v>
       </c>
-      <c r="D1" s="25">
+      <c r="D1" s="21">
         <v>3</v>
       </c>
-      <c r="E1" s="25">
+      <c r="E1" s="21">
         <v>4</v>
       </c>
-      <c r="F1" s="25">
+      <c r="F1" s="21">
         <v>5</v>
       </c>
-      <c r="G1" s="25">
+      <c r="G1" s="21">
         <v>6</v>
       </c>
-      <c r="H1" s="25">
+      <c r="H1" s="21">
         <v>7</v>
       </c>
-      <c r="I1" s="25">
-        <v>8</v>
-      </c>
-      <c r="J1" s="25">
+      <c r="I1" s="21">
+        <v>8</v>
+      </c>
+      <c r="J1" s="21">
         <v>11</v>
       </c>
-      <c r="K1" s="25">
+      <c r="K1" s="21">
         <v>13</v>
       </c>
-      <c r="L1" s="25">
-        <v>14</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>537</v>
-      </c>
-      <c r="N1" s="26" t="s">
+      <c r="L1" s="21">
+        <v>14</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>535</v>
+      </c>
+      <c r="N1" s="22" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="24" t="s">
+      <c r="B2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="36" t="s">
         <v>3</v>
       </c>
       <c r="N2" s="5" t="s">
@@ -2416,8 +2436,8 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="55" t="s">
-        <v>539</v>
+      <c r="M3" s="48" t="s">
+        <v>537</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>8</v>
@@ -2440,7 +2460,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="37" t="s">
         <v>503</v>
       </c>
       <c r="N4" s="5" t="s">
@@ -2464,7 +2484,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="20" t="s">
+      <c r="M5" s="37" t="s">
         <v>504</v>
       </c>
       <c r="N5" s="5" t="s">
@@ -2488,7 +2508,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="37" t="s">
         <v>505</v>
       </c>
       <c r="N6" s="5" t="s">
@@ -2516,8 +2536,8 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="21" t="s">
-        <v>517</v>
+      <c r="M7" s="38" t="s">
+        <v>516</v>
       </c>
       <c r="N7" s="5" t="s">
         <v>8</v>
@@ -2540,7 +2560,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="20" t="s">
+      <c r="M8" s="37" t="s">
         <v>506</v>
       </c>
       <c r="N8" s="5" t="s">
@@ -2570,8 +2590,8 @@
       </c>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
-      <c r="M9" s="31" t="s">
-        <v>512</v>
+      <c r="M9" s="39" t="s">
+        <v>511</v>
       </c>
       <c r="N9" s="5" t="s">
         <v>8</v>
@@ -2594,7 +2614,7 @@
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
-      <c r="M10" s="31"/>
+      <c r="M10" s="39"/>
       <c r="N10" s="5" t="s">
         <v>8</v>
       </c>
@@ -2616,7 +2636,7 @@
       <c r="J11" s="16"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
-      <c r="M11" s="31"/>
+      <c r="M11" s="39"/>
       <c r="N11" s="5" t="s">
         <v>8</v>
       </c>
@@ -2638,7 +2658,7 @@
       <c r="J12" s="16"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
-      <c r="M12" s="31"/>
+      <c r="M12" s="39"/>
       <c r="N12" s="5" t="s">
         <v>8</v>
       </c>
@@ -2660,7 +2680,7 @@
         <v>8</v>
       </c>
       <c r="L13" s="17"/>
-      <c r="M13" s="31"/>
+      <c r="M13" s="39"/>
       <c r="N13" s="5" t="s">
         <v>8</v>
       </c>
@@ -2682,8 +2702,8 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="20" t="s">
-        <v>515</v>
+      <c r="M14" s="37" t="s">
+        <v>514</v>
       </c>
       <c r="N14" s="5" t="s">
         <v>8</v>
@@ -2706,8 +2726,8 @@
       <c r="J15" s="1"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="20" t="s">
-        <v>515</v>
+      <c r="M15" s="37" t="s">
+        <v>514</v>
       </c>
       <c r="N15" s="5" t="s">
         <v>8</v>
@@ -2730,8 +2750,8 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="21" t="s">
-        <v>513</v>
+      <c r="M16" s="38" t="s">
+        <v>512</v>
       </c>
       <c r="N16" s="5" t="s">
         <v>8</v>
@@ -2754,8 +2774,8 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="21" t="s">
-        <v>516</v>
+      <c r="M17" s="38" t="s">
+        <v>515</v>
       </c>
       <c r="N17" s="5" t="s">
         <v>8</v>
@@ -2778,8 +2798,8 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="20" t="s">
-        <v>518</v>
+      <c r="M18" s="37" t="s">
+        <v>517</v>
       </c>
       <c r="N18" s="5" t="s">
         <v>8</v>
@@ -2802,8 +2822,8 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="20" t="s">
-        <v>519</v>
+      <c r="M19" s="37" t="s">
+        <v>518</v>
       </c>
       <c r="N19" s="5" t="s">
         <v>8</v>
@@ -2826,8 +2846,8 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="32" t="s">
-        <v>514</v>
+      <c r="M20" s="40" t="s">
+        <v>513</v>
       </c>
       <c r="N20" s="5" t="s">
         <v>8</v>
@@ -2850,7 +2870,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="33"/>
+      <c r="M21" s="41"/>
       <c r="N21" s="5" t="s">
         <v>8</v>
       </c>
@@ -2872,8 +2892,8 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="48" t="s">
-        <v>530</v>
+      <c r="M22" s="49" t="s">
+        <v>529</v>
       </c>
       <c r="N22" s="5" t="s">
         <v>8</v>
@@ -2894,8 +2914,8 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="20" t="s">
-        <v>520</v>
+      <c r="M23" s="37" t="s">
+        <v>519</v>
       </c>
       <c r="N23" s="5" t="s">
         <v>8</v>
@@ -2918,8 +2938,8 @@
         <v>8</v>
       </c>
       <c r="L24" s="1"/>
-      <c r="M24" s="48" t="s">
-        <v>520</v>
+      <c r="M24" s="49" t="s">
+        <v>519</v>
       </c>
       <c r="N24" s="5" t="s">
         <v>8</v>
@@ -2942,8 +2962,8 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-      <c r="M25" s="20" t="s">
-        <v>522</v>
+      <c r="M25" s="37" t="s">
+        <v>521</v>
       </c>
       <c r="N25" s="5" t="s">
         <v>8</v>
@@ -2966,8 +2986,8 @@
       <c r="J26" s="17"/>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
-      <c r="M26" s="29" t="s">
-        <v>521</v>
+      <c r="M26" s="42" t="s">
+        <v>520</v>
       </c>
       <c r="N26" s="5" t="s">
         <v>8</v>
@@ -2990,7 +3010,7 @@
       <c r="J27" s="17"/>
       <c r="K27" s="17"/>
       <c r="L27" s="17"/>
-      <c r="M27" s="34"/>
+      <c r="M27" s="43"/>
       <c r="N27" s="5" t="s">
         <v>8</v>
       </c>
@@ -3012,7 +3032,7 @@
       <c r="J28" s="17"/>
       <c r="K28" s="17"/>
       <c r="L28" s="17"/>
-      <c r="M28" s="34"/>
+      <c r="M28" s="43"/>
       <c r="N28" s="5" t="s">
         <v>8</v>
       </c>
@@ -3034,7 +3054,7 @@
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
       <c r="L29" s="17"/>
-      <c r="M29" s="30"/>
+      <c r="M29" s="44"/>
       <c r="N29" s="5" t="s">
         <v>8</v>
       </c>
@@ -3056,8 +3076,8 @@
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="28" t="s">
-        <v>529</v>
+      <c r="M30" s="45" t="s">
+        <v>528</v>
       </c>
       <c r="N30" s="5" t="s">
         <v>8</v>
@@ -3082,8 +3102,8 @@
       <c r="L31" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="29" t="s">
-        <v>523</v>
+      <c r="M31" s="42" t="s">
+        <v>522</v>
       </c>
       <c r="N31" s="5" t="s">
         <v>8</v>
@@ -3106,7 +3126,7 @@
       <c r="L32" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="30"/>
+      <c r="M32" s="44"/>
       <c r="N32" s="5" t="s">
         <v>8</v>
       </c>
@@ -3128,8 +3148,8 @@
       <c r="L33" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="M33" s="20" t="s">
-        <v>524</v>
+      <c r="M33" s="37" t="s">
+        <v>523</v>
       </c>
       <c r="N33" s="5" t="s">
         <v>8</v>
@@ -3152,8 +3172,8 @@
       <c r="L34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M34" s="20" t="s">
-        <v>525</v>
+      <c r="M34" s="37" t="s">
+        <v>524</v>
       </c>
       <c r="N34" s="5" t="s">
         <v>8</v>
@@ -3176,8 +3196,8 @@
       <c r="L35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M35" s="29" t="s">
-        <v>528</v>
+      <c r="M35" s="42" t="s">
+        <v>527</v>
       </c>
       <c r="N35" s="5" t="s">
         <v>8</v>
@@ -3200,7 +3220,7 @@
       <c r="L36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M36" s="30"/>
+      <c r="M36" s="44"/>
       <c r="N36" s="5" t="s">
         <v>8</v>
       </c>
@@ -3222,8 +3242,8 @@
       <c r="L37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M37" s="20" t="s">
-        <v>527</v>
+      <c r="M37" s="37" t="s">
+        <v>526</v>
       </c>
       <c r="N37" s="5" t="s">
         <v>8</v>
@@ -3246,8 +3266,8 @@
       <c r="L38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M38" s="20" t="s">
-        <v>524</v>
+      <c r="M38" s="37" t="s">
+        <v>523</v>
       </c>
       <c r="N38" s="5" t="s">
         <v>8</v>
@@ -3292,8 +3312,8 @@
       </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
-      <c r="M40" s="49" t="s">
-        <v>536</v>
+      <c r="M40" s="50" t="s">
+        <v>534</v>
       </c>
       <c r="N40" s="5" t="s">
         <v>8</v>
@@ -3316,7 +3336,7 @@
       </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
-      <c r="M41" s="50"/>
+      <c r="M41" s="51"/>
       <c r="N41" s="5" t="s">
         <v>8</v>
       </c>
@@ -3338,19 +3358,19 @@
       </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="51"/>
+      <c r="M42" s="52"/>
       <c r="N42" s="5" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="M40:M42"/>
     <mergeCell ref="M35:M36"/>
     <mergeCell ref="M9:M13"/>
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="M26:M29"/>
     <mergeCell ref="M31:M32"/>
-    <mergeCell ref="M40:M42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3362,8 +3382,8 @@
   <dimension ref="A1:G292"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G162" sqref="G162"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3378,30 +3398,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="46" t="s">
-        <v>538</v>
+      <c r="G1" s="24" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1"/>
@@ -3418,7 +3438,7 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="36"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="1" t="s">
         <v>69</v>
       </c>
@@ -3435,7 +3455,7 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="36"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
@@ -3448,7 +3468,7 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="1" t="s">
         <v>73</v>
       </c>
@@ -3463,7 +3483,7 @@
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="1" t="s">
         <v>76</v>
       </c>
@@ -3480,7 +3500,7 @@
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="1" t="s">
         <v>77</v>
       </c>
@@ -3495,7 +3515,7 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="1" t="s">
         <v>79</v>
       </c>
@@ -3510,7 +3530,7 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="1" t="s">
         <v>80</v>
       </c>
@@ -3525,7 +3545,7 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>84</v>
       </c>
@@ -3540,7 +3560,7 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>85</v>
       </c>
@@ -3555,7 +3575,7 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>89</v>
       </c>
@@ -3570,7 +3590,7 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="1" t="s">
         <v>91</v>
       </c>
@@ -3585,7 +3605,7 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="1" t="s">
         <v>93</v>
       </c>
@@ -3600,7 +3620,7 @@
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="36"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="1" t="s">
         <v>95</v>
       </c>
@@ -3615,7 +3635,7 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>97</v>
       </c>
@@ -3630,7 +3650,7 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
@@ -3645,7 +3665,7 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="1" t="s">
         <v>103</v>
       </c>
@@ -3658,7 +3678,7 @@
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="1" t="s">
         <v>104</v>
       </c>
@@ -3671,7 +3691,7 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="36"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="1" t="s">
         <v>105</v>
       </c>
@@ -3684,7 +3704,7 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="1" t="s">
         <v>106</v>
       </c>
@@ -3697,7 +3717,7 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="1" t="s">
         <v>107</v>
       </c>
@@ -3710,7 +3730,7 @@
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="36"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="1" t="s">
         <v>108</v>
       </c>
@@ -3723,7 +3743,7 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
+      <c r="A24" s="31"/>
       <c r="B24" s="1" t="s">
         <v>109</v>
       </c>
@@ -3736,7 +3756,7 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="1" t="s">
         <v>60</v>
       </c>
@@ -3749,7 +3769,7 @@
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="1" t="s">
         <v>110</v>
       </c>
@@ -3762,7 +3782,7 @@
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="36"/>
+      <c r="A27" s="31"/>
       <c r="B27" s="1" t="s">
         <v>111</v>
       </c>
@@ -3775,7 +3795,7 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="37"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="1" t="s">
         <v>112</v>
       </c>
@@ -3788,7 +3808,7 @@
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="28" t="s">
         <v>53</v>
       </c>
       <c r="B29" s="1"/>
@@ -3801,7 +3821,7 @@
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="36"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="1" t="s">
         <v>69</v>
       </c>
@@ -3816,7 +3836,7 @@
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="36"/>
+      <c r="A31" s="31"/>
       <c r="B31" s="1" t="s">
         <v>72</v>
       </c>
@@ -3831,7 +3851,7 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="36"/>
+      <c r="A32" s="31"/>
       <c r="B32" s="1" t="s">
         <v>118</v>
       </c>
@@ -3846,7 +3866,7 @@
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="3" t="s">
         <v>120</v>
       </c>
@@ -3861,7 +3881,7 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="36"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="1" t="s">
         <v>84</v>
       </c>
@@ -3876,7 +3896,7 @@
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="36"/>
+      <c r="A35" s="31"/>
       <c r="B35" s="1" t="s">
         <v>123</v>
       </c>
@@ -3891,7 +3911,7 @@
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="36"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="1" t="s">
         <v>125</v>
       </c>
@@ -3906,7 +3926,7 @@
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="36"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="1" t="s">
         <v>127</v>
       </c>
@@ -3921,7 +3941,7 @@
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="36"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="1" t="s">
         <v>129</v>
       </c>
@@ -3936,7 +3956,7 @@
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="36"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="1" t="s">
         <v>131</v>
       </c>
@@ -3951,7 +3971,7 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="36"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="1" t="s">
         <v>133</v>
       </c>
@@ -3966,7 +3986,7 @@
       <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="36"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="1" t="s">
         <v>135</v>
       </c>
@@ -3981,7 +4001,7 @@
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="36"/>
+      <c r="A42" s="31"/>
       <c r="B42" s="1" t="s">
         <v>137</v>
       </c>
@@ -3996,7 +4016,7 @@
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="36"/>
+      <c r="A43" s="31"/>
       <c r="B43" s="1" t="s">
         <v>139</v>
       </c>
@@ -4011,7 +4031,7 @@
       <c r="G43" s="1"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="36"/>
+      <c r="A44" s="31"/>
       <c r="B44" s="1" t="s">
         <v>141</v>
       </c>
@@ -4026,7 +4046,7 @@
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="36"/>
+      <c r="A45" s="31"/>
       <c r="B45" s="1" t="s">
         <v>143</v>
       </c>
@@ -4041,7 +4061,7 @@
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="36"/>
+      <c r="A46" s="31"/>
       <c r="B46" s="1" t="s">
         <v>145</v>
       </c>
@@ -4056,7 +4076,7 @@
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="36"/>
+      <c r="A47" s="31"/>
       <c r="B47" s="1" t="s">
         <v>147</v>
       </c>
@@ -4071,7 +4091,7 @@
       <c r="G47" s="1"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="36"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="1" t="s">
         <v>149</v>
       </c>
@@ -4086,7 +4106,7 @@
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="36"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="1" t="s">
         <v>151</v>
       </c>
@@ -4101,7 +4121,7 @@
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="36"/>
+      <c r="A50" s="31"/>
       <c r="B50" s="1" t="s">
         <v>153</v>
       </c>
@@ -4116,7 +4136,7 @@
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="36"/>
+      <c r="A51" s="31"/>
       <c r="B51" s="1" t="s">
         <v>155</v>
       </c>
@@ -4131,7 +4151,7 @@
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="36"/>
+      <c r="A52" s="31"/>
       <c r="B52" s="1" t="s">
         <v>157</v>
       </c>
@@ -4146,7 +4166,7 @@
       <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="36"/>
+      <c r="A53" s="31"/>
       <c r="B53" s="1" t="s">
         <v>159</v>
       </c>
@@ -4161,7 +4181,7 @@
       <c r="G53" s="1"/>
     </row>
     <row r="54" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="37"/>
+      <c r="A54" s="29"/>
       <c r="B54" s="1" t="s">
         <v>161</v>
       </c>
@@ -4176,7 +4196,7 @@
       <c r="G54" s="1"/>
     </row>
     <row r="55" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B55" s="1"/>
@@ -4191,7 +4211,7 @@
       <c r="G55" s="1"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="36"/>
+      <c r="A56" s="31"/>
       <c r="B56" s="1" t="s">
         <v>163</v>
       </c>
@@ -4204,7 +4224,7 @@
       <c r="G56" s="1"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="36"/>
+      <c r="A57" s="31"/>
       <c r="B57" s="1" t="s">
         <v>164</v>
       </c>
@@ -4221,7 +4241,7 @@
       <c r="G57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="36"/>
+      <c r="A58" s="31"/>
       <c r="B58" s="1" t="s">
         <v>165</v>
       </c>
@@ -4238,7 +4258,7 @@
       <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="36"/>
+      <c r="A59" s="31"/>
       <c r="B59" s="1" t="s">
         <v>166</v>
       </c>
@@ -4255,7 +4275,7 @@
       <c r="G59" s="1"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="37"/>
+      <c r="A60" s="29"/>
       <c r="B60" s="1" t="s">
         <v>167</v>
       </c>
@@ -4268,7 +4288,7 @@
       <c r="G60" s="1"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="38" t="s">
+      <c r="A61" s="34" t="s">
         <v>5</v>
       </c>
       <c r="B61" s="3"/>
@@ -4283,7 +4303,7 @@
       <c r="G61" s="1"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="38"/>
+      <c r="A62" s="34"/>
       <c r="B62" s="3" t="s">
         <v>169</v>
       </c>
@@ -4296,7 +4316,7 @@
       <c r="G62" s="1"/>
     </row>
     <row r="63" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="38"/>
+      <c r="A63" s="34"/>
       <c r="B63" s="3" t="s">
         <v>170</v>
       </c>
@@ -4313,7 +4333,7 @@
       <c r="G63" s="1"/>
     </row>
     <row r="64" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A64" s="38"/>
+      <c r="A64" s="34"/>
       <c r="B64" s="3" t="s">
         <v>171</v>
       </c>
@@ -4330,7 +4350,7 @@
       <c r="G64" s="1"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="38"/>
+      <c r="A65" s="34"/>
       <c r="B65" s="3" t="s">
         <v>172</v>
       </c>
@@ -4362,7 +4382,7 @@
       <c r="G66" s="1"/>
     </row>
     <row r="67" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A67" s="39" t="s">
+      <c r="A67" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B67" s="3"/>
@@ -4379,7 +4399,7 @@
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A68" s="39"/>
+      <c r="A68" s="32"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3" t="s">
         <v>185</v>
@@ -4392,7 +4412,7 @@
       <c r="G68" s="1"/>
     </row>
     <row r="69" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A69" s="39"/>
+      <c r="A69" s="32"/>
       <c r="B69" s="3" t="s">
         <v>180</v>
       </c>
@@ -4407,7 +4427,7 @@
       <c r="G69" s="1"/>
     </row>
     <row r="70" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="39"/>
+      <c r="A70" s="32"/>
       <c r="B70" s="3" t="s">
         <v>181</v>
       </c>
@@ -4422,7 +4442,7 @@
       <c r="G70" s="1"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="39"/>
+      <c r="A71" s="32"/>
       <c r="B71" s="3" t="s">
         <v>182</v>
       </c>
@@ -4437,7 +4457,7 @@
       <c r="G71" s="1"/>
     </row>
     <row r="72" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="39"/>
+      <c r="A72" s="32"/>
       <c r="B72" s="3" t="s">
         <v>186</v>
       </c>
@@ -4452,7 +4472,7 @@
       <c r="G72" s="1"/>
     </row>
     <row r="73" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="39"/>
+      <c r="A73" s="32"/>
       <c r="B73" s="3" t="s">
         <v>188</v>
       </c>
@@ -4465,7 +4485,7 @@
       <c r="G73" s="1"/>
     </row>
     <row r="74" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="39"/>
+      <c r="A74" s="32"/>
       <c r="B74" s="3" t="s">
         <v>189</v>
       </c>
@@ -4482,7 +4502,7 @@
       <c r="G74" s="1"/>
     </row>
     <row r="75" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A75" s="39"/>
+      <c r="A75" s="32"/>
       <c r="B75" s="3" t="s">
         <v>192</v>
       </c>
@@ -4499,7 +4519,7 @@
       <c r="G75" s="1"/>
     </row>
     <row r="76" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A76" s="39"/>
+      <c r="A76" s="32"/>
       <c r="B76" s="3" t="s">
         <v>195</v>
       </c>
@@ -4516,7 +4536,7 @@
       <c r="G76" s="1"/>
     </row>
     <row r="77" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="39"/>
+      <c r="A77" s="32"/>
       <c r="B77" s="3" t="s">
         <v>198</v>
       </c>
@@ -4531,7 +4551,7 @@
       <c r="G77" s="1"/>
     </row>
     <row r="78" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A78" s="39"/>
+      <c r="A78" s="32"/>
       <c r="B78" s="3" t="s">
         <v>200</v>
       </c>
@@ -4548,7 +4568,7 @@
       <c r="G78" s="1"/>
     </row>
     <row r="79" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="39"/>
+      <c r="A79" s="32"/>
       <c r="B79" s="3" t="s">
         <v>202</v>
       </c>
@@ -4565,7 +4585,7 @@
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="39"/>
+      <c r="A80" s="32"/>
       <c r="B80" s="3" t="s">
         <v>205</v>
       </c>
@@ -4582,7 +4602,7 @@
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A81" s="39"/>
+      <c r="A81" s="32"/>
       <c r="B81" s="3" t="s">
         <v>208</v>
       </c>
@@ -4599,7 +4619,7 @@
       <c r="G81" s="1"/>
     </row>
     <row r="82" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A82" s="35" t="s">
+      <c r="A82" s="28" t="s">
         <v>44</v>
       </c>
       <c r="B82" s="3"/>
@@ -4616,7 +4636,7 @@
       <c r="G82" s="1"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="37"/>
+      <c r="A83" s="29"/>
       <c r="B83" s="3" t="s">
         <v>288</v>
       </c>
@@ -4629,7 +4649,7 @@
       <c r="G83" s="1"/>
     </row>
     <row r="84" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A84" s="42" t="s">
+      <c r="A84" s="27" t="s">
         <v>282</v>
       </c>
       <c r="B84" s="1"/>
@@ -4644,7 +4664,7 @@
       <c r="G84" s="1"/>
     </row>
     <row r="85" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A85" s="42"/>
+      <c r="A85" s="27"/>
       <c r="B85" s="1"/>
       <c r="C85" s="3" t="s">
         <v>219</v>
@@ -4659,7 +4679,7 @@
       <c r="G85" s="1"/>
     </row>
     <row r="86" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="42"/>
+      <c r="A86" s="27"/>
       <c r="B86" s="1"/>
       <c r="C86" s="3" t="s">
         <v>229</v>
@@ -4672,7 +4692,7 @@
       <c r="G86" s="1"/>
     </row>
     <row r="87" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A87" s="42"/>
+      <c r="A87" s="27"/>
       <c r="B87" s="1"/>
       <c r="C87" s="3" t="s">
         <v>279</v>
@@ -4685,7 +4705,7 @@
       <c r="G87" s="1"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" s="42"/>
+      <c r="A88" s="27"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
         <v>281</v>
@@ -4698,7 +4718,7 @@
       <c r="G88" s="1"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A89" s="42"/>
+      <c r="A89" s="27"/>
       <c r="B89" s="3" t="s">
         <v>180</v>
       </c>
@@ -4711,7 +4731,7 @@
       <c r="G89" s="1"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A90" s="42"/>
+      <c r="A90" s="27"/>
       <c r="B90" s="3" t="s">
         <v>181</v>
       </c>
@@ -4724,7 +4744,7 @@
       <c r="G90" s="1"/>
     </row>
     <row r="91" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A91" s="42"/>
+      <c r="A91" s="27"/>
       <c r="B91" s="3" t="s">
         <v>230</v>
       </c>
@@ -4737,7 +4757,7 @@
       <c r="G91" s="1"/>
     </row>
     <row r="92" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A92" s="42"/>
+      <c r="A92" s="27"/>
       <c r="B92" s="9" t="s">
         <v>218</v>
       </c>
@@ -4752,7 +4772,7 @@
       <c r="G92" s="1"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="42"/>
+      <c r="A93" s="27"/>
       <c r="B93" s="3" t="s">
         <v>9</v>
       </c>
@@ -4767,7 +4787,7 @@
       <c r="G93" s="1"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A94" s="42"/>
+      <c r="A94" s="27"/>
       <c r="B94" s="3" t="s">
         <v>215</v>
       </c>
@@ -4782,7 +4802,7 @@
       <c r="G94" s="1"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A95" s="42"/>
+      <c r="A95" s="27"/>
       <c r="B95" s="3" t="s">
         <v>216</v>
       </c>
@@ -4795,7 +4815,7 @@
       <c r="G95" s="1"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A96" s="42"/>
+      <c r="A96" s="27"/>
       <c r="B96" s="3" t="s">
         <v>221</v>
       </c>
@@ -4810,7 +4830,7 @@
       <c r="G96" s="1"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A97" s="42"/>
+      <c r="A97" s="27"/>
       <c r="B97" s="3" t="s">
         <v>223</v>
       </c>
@@ -4825,7 +4845,7 @@
       <c r="G97" s="1"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A98" s="42"/>
+      <c r="A98" s="27"/>
       <c r="B98" s="3" t="s">
         <v>225</v>
       </c>
@@ -4840,7 +4860,7 @@
       <c r="G98" s="1"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A99" s="42"/>
+      <c r="A99" s="27"/>
       <c r="B99" s="3" t="s">
         <v>227</v>
       </c>
@@ -4870,7 +4890,7 @@
       <c r="G100" s="1"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A101" s="35" t="s">
+      <c r="A101" s="28" t="s">
         <v>59</v>
       </c>
       <c r="B101" s="3"/>
@@ -4885,7 +4905,7 @@
       <c r="G101" s="1"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" s="36"/>
+      <c r="A102" s="31"/>
       <c r="B102" s="3" t="s">
         <v>284</v>
       </c>
@@ -4896,7 +4916,7 @@
       <c r="G102" s="1"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A103" s="36"/>
+      <c r="A103" s="31"/>
       <c r="B103" s="3" t="s">
         <v>285</v>
       </c>
@@ -4907,7 +4927,7 @@
       <c r="G103" s="1"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A104" s="37"/>
+      <c r="A104" s="29"/>
       <c r="B104" s="3" t="s">
         <v>286</v>
       </c>
@@ -4918,7 +4938,7 @@
       <c r="G104" s="1"/>
     </row>
     <row r="105" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A105" s="42" t="s">
+      <c r="A105" s="27" t="s">
         <v>10</v>
       </c>
       <c r="B105" s="1"/>
@@ -4935,7 +4955,7 @@
       <c r="G105" s="1"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" s="42"/>
+      <c r="A106" s="27"/>
       <c r="B106" s="3" t="s">
         <v>232</v>
       </c>
@@ -4950,7 +4970,7 @@
       <c r="G106" s="1"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A107" s="42"/>
+      <c r="A107" s="27"/>
       <c r="B107" s="3" t="s">
         <v>233</v>
       </c>
@@ -4967,7 +4987,7 @@
       <c r="G107" s="1"/>
     </row>
     <row r="108" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="42" t="s">
+      <c r="A108" s="27" t="s">
         <v>11</v>
       </c>
       <c r="B108" s="1"/>
@@ -4982,7 +5002,7 @@
       <c r="G108" s="1"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A109" s="42"/>
+      <c r="A109" s="27"/>
       <c r="B109" s="3" t="s">
         <v>234</v>
       </c>
@@ -4997,7 +5017,7 @@
       <c r="G109" s="1"/>
     </row>
     <row r="110" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A110" s="42" t="s">
+      <c r="A110" s="27" t="s">
         <v>236</v>
       </c>
       <c r="B110" s="1"/>
@@ -5016,7 +5036,7 @@
       <c r="G110" s="1"/>
     </row>
     <row r="111" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A111" s="42"/>
+      <c r="A111" s="27"/>
       <c r="B111" s="3" t="s">
         <v>240</v>
       </c>
@@ -5031,7 +5051,7 @@
       <c r="G111" s="1"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A112" s="42"/>
+      <c r="A112" s="27"/>
       <c r="B112" s="1" t="s">
         <v>242</v>
       </c>
@@ -5048,7 +5068,7 @@
       <c r="G112" s="1"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A113" s="42"/>
+      <c r="A113" s="27"/>
       <c r="B113" s="3" t="s">
         <v>244</v>
       </c>
@@ -5065,7 +5085,7 @@
       <c r="G113" s="1"/>
     </row>
     <row r="114" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A114" s="42"/>
+      <c r="A114" s="27"/>
       <c r="B114" s="1" t="s">
         <v>245</v>
       </c>
@@ -5084,7 +5104,7 @@
       <c r="G114" s="1"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A115" s="42"/>
+      <c r="A115" s="27"/>
       <c r="B115" s="3" t="s">
         <v>247</v>
       </c>
@@ -5099,7 +5119,7 @@
       <c r="G115" s="1"/>
     </row>
     <row r="116" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A116" s="42" t="s">
+      <c r="A116" s="27" t="s">
         <v>13</v>
       </c>
       <c r="B116" s="1"/>
@@ -5114,7 +5134,7 @@
       <c r="G116" s="1"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A117" s="42"/>
+      <c r="A117" s="27"/>
       <c r="B117" s="3" t="s">
         <v>250</v>
       </c>
@@ -5127,7 +5147,7 @@
       <c r="G117" s="1"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A118" s="42" t="s">
+      <c r="A118" s="27" t="s">
         <v>14</v>
       </c>
       <c r="B118" s="1"/>
@@ -5142,7 +5162,7 @@
       <c r="G118" s="1"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A119" s="42"/>
+      <c r="A119" s="27"/>
       <c r="B119" s="3" t="s">
         <v>252</v>
       </c>
@@ -5155,7 +5175,7 @@
       <c r="G119" s="1"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A120" s="42"/>
+      <c r="A120" s="27"/>
       <c r="B120" s="1" t="s">
         <v>253</v>
       </c>
@@ -5168,7 +5188,7 @@
       <c r="G120" s="1"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A121" s="42"/>
+      <c r="A121" s="27"/>
       <c r="B121" s="3" t="s">
         <v>254</v>
       </c>
@@ -5183,7 +5203,7 @@
       <c r="G121" s="1"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A122" s="42"/>
+      <c r="A122" s="27"/>
       <c r="B122" s="1" t="s">
         <v>256</v>
       </c>
@@ -5198,7 +5218,7 @@
       <c r="G122" s="1"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A123" s="42" t="s">
+      <c r="A123" s="27" t="s">
         <v>15</v>
       </c>
       <c r="B123" s="1"/>
@@ -5213,7 +5233,7 @@
       <c r="G123" s="1"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A124" s="42"/>
+      <c r="A124" s="27"/>
       <c r="B124" s="1" t="s">
         <v>259</v>
       </c>
@@ -5226,7 +5246,7 @@
       <c r="G124" s="1"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A125" s="42"/>
+      <c r="A125" s="27"/>
       <c r="B125" s="1" t="s">
         <v>253</v>
       </c>
@@ -5241,7 +5261,7 @@
       <c r="G125" s="1"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A126" s="42"/>
+      <c r="A126" s="27"/>
       <c r="B126" s="1" t="s">
         <v>254</v>
       </c>
@@ -5256,7 +5276,7 @@
       <c r="G126" s="1"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A127" s="42"/>
+      <c r="A127" s="27"/>
       <c r="B127" s="1" t="s">
         <v>256</v>
       </c>
@@ -5271,7 +5291,7 @@
       <c r="G127" s="1"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A128" s="42"/>
+      <c r="A128" s="27"/>
       <c r="B128" s="1" t="s">
         <v>263</v>
       </c>
@@ -5286,7 +5306,7 @@
       <c r="G128" s="1"/>
     </row>
     <row r="129" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="35" t="s">
+      <c r="A129" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B129" s="1"/>
@@ -5303,7 +5323,7 @@
       <c r="G129" s="1"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A130" s="36"/>
+      <c r="A130" s="31"/>
       <c r="B130" s="1" t="s">
         <v>267</v>
       </c>
@@ -5318,7 +5338,7 @@
       <c r="G130" s="1"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A131" s="36"/>
+      <c r="A131" s="31"/>
       <c r="B131" s="1" t="s">
         <v>269</v>
       </c>
@@ -5331,7 +5351,7 @@
       <c r="G131" s="1"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A132" s="36"/>
+      <c r="A132" s="31"/>
       <c r="B132" s="1" t="s">
         <v>125</v>
       </c>
@@ -5344,7 +5364,7 @@
       <c r="G132" s="1"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A133" s="36"/>
+      <c r="A133" s="31"/>
       <c r="B133" s="1" t="s">
         <v>270</v>
       </c>
@@ -5357,7 +5377,7 @@
       <c r="G133" s="1"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A134" s="36"/>
+      <c r="A134" s="31"/>
       <c r="B134" s="1" t="s">
         <v>271</v>
       </c>
@@ -5370,7 +5390,7 @@
       <c r="G134" s="1"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A135" s="36"/>
+      <c r="A135" s="31"/>
       <c r="B135" s="1" t="s">
         <v>272</v>
       </c>
@@ -5383,7 +5403,7 @@
       <c r="G135" s="1"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A136" s="36"/>
+      <c r="A136" s="31"/>
       <c r="B136" s="1" t="s">
         <v>273</v>
       </c>
@@ -5396,7 +5416,7 @@
       <c r="G136" s="1"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A137" s="36"/>
+      <c r="A137" s="31"/>
       <c r="B137" s="1" t="s">
         <v>274</v>
       </c>
@@ -5409,7 +5429,7 @@
       <c r="G137" s="1"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A138" s="36"/>
+      <c r="A138" s="31"/>
       <c r="B138" s="1" t="s">
         <v>275</v>
       </c>
@@ -5422,7 +5442,7 @@
       <c r="G138" s="1"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A139" s="37"/>
+      <c r="A139" s="29"/>
       <c r="B139" s="1" t="s">
         <v>276</v>
       </c>
@@ -5435,7 +5455,7 @@
       <c r="G139" s="1"/>
     </row>
     <row r="140" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="40" t="s">
+      <c r="A140" s="35" t="s">
         <v>17</v>
       </c>
       <c r="B140" s="1"/>
@@ -5450,7 +5470,7 @@
       <c r="G140" s="1"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A141" s="41"/>
+      <c r="A141" s="26"/>
       <c r="B141" s="1" t="s">
         <v>278</v>
       </c>
@@ -5463,7 +5483,7 @@
       <c r="G141" s="1"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A142" s="35" t="s">
+      <c r="A142" s="28" t="s">
         <v>27</v>
       </c>
       <c r="B142" s="1"/>
@@ -5475,12 +5495,12 @@
       <c r="F142" s="1">
         <v>5</v>
       </c>
-      <c r="G142" s="55" t="s">
-        <v>531</v>
+      <c r="G142" s="48" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A143" s="36"/>
+      <c r="A143" s="31"/>
       <c r="B143" s="3" t="s">
         <v>20</v>
       </c>
@@ -5493,7 +5513,7 @@
       <c r="G143" s="1"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A144" s="36"/>
+      <c r="A144" s="31"/>
       <c r="B144" s="1" t="s">
         <v>21</v>
       </c>
@@ -5506,7 +5526,7 @@
       <c r="G144" s="1"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A145" s="36"/>
+      <c r="A145" s="31"/>
       <c r="B145" s="1" t="s">
         <v>22</v>
       </c>
@@ -5519,7 +5539,7 @@
       <c r="G145" s="1"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A146" s="36"/>
+      <c r="A146" s="31"/>
       <c r="B146" s="1" t="s">
         <v>23</v>
       </c>
@@ -5532,7 +5552,7 @@
       <c r="G146" s="1"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A147" s="36"/>
+      <c r="A147" s="31"/>
       <c r="B147" s="1" t="s">
         <v>24</v>
       </c>
@@ -5545,7 +5565,7 @@
       <c r="G147" s="1"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A148" s="36"/>
+      <c r="A148" s="31"/>
       <c r="B148" s="1" t="s">
         <v>25</v>
       </c>
@@ -5558,7 +5578,7 @@
       <c r="G148" s="1"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A149" s="36"/>
+      <c r="A149" s="31"/>
       <c r="B149" s="1" t="s">
         <v>26</v>
       </c>
@@ -5571,7 +5591,7 @@
       <c r="G149" s="1"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A150" s="36"/>
+      <c r="A150" s="31"/>
       <c r="B150" s="1" t="s">
         <v>32</v>
       </c>
@@ -5584,7 +5604,7 @@
       <c r="G150" s="1"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A151" s="36"/>
+      <c r="A151" s="31"/>
       <c r="B151" s="1" t="s">
         <v>33</v>
       </c>
@@ -5597,7 +5617,7 @@
       <c r="G151" s="1"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A152" s="36"/>
+      <c r="A152" s="31"/>
       <c r="B152" s="1" t="s">
         <v>35</v>
       </c>
@@ -5610,7 +5630,7 @@
       <c r="G152" s="1"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A153" s="36"/>
+      <c r="A153" s="31"/>
       <c r="B153" s="1" t="s">
         <v>36</v>
       </c>
@@ -5623,7 +5643,7 @@
       <c r="G153" s="1"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A154" s="37"/>
+      <c r="A154" s="29"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
@@ -5634,7 +5654,7 @@
       <c r="G154" s="1"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A155" s="35" t="s">
+      <c r="A155" s="28" t="s">
         <v>29</v>
       </c>
       <c r="B155" s="1"/>
@@ -5646,12 +5666,12 @@
       <c r="F155" s="1">
         <v>5</v>
       </c>
-      <c r="G155" s="55" t="s">
-        <v>532</v>
+      <c r="G155" s="48" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A156" s="36"/>
+      <c r="A156" s="31"/>
       <c r="B156" s="1" t="s">
         <v>30</v>
       </c>
@@ -5664,7 +5684,7 @@
       <c r="G156" s="1"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A157" s="36"/>
+      <c r="A157" s="31"/>
       <c r="B157" s="1" t="s">
         <v>37</v>
       </c>
@@ -5677,7 +5697,7 @@
       <c r="G157" s="1"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A158" s="36"/>
+      <c r="A158" s="31"/>
       <c r="B158" s="1" t="s">
         <v>40</v>
       </c>
@@ -5690,7 +5710,7 @@
       <c r="G158" s="1"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A159" s="36"/>
+      <c r="A159" s="31"/>
       <c r="B159" s="1" t="s">
         <v>41</v>
       </c>
@@ -5705,7 +5725,7 @@
       <c r="G159" s="1"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A160" s="36"/>
+      <c r="A160" s="31"/>
       <c r="B160" s="1" t="s">
         <v>39</v>
       </c>
@@ -5720,7 +5740,7 @@
       <c r="G160" s="1"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A161" s="37"/>
+      <c r="A161" s="29"/>
       <c r="B161" s="1" t="s">
         <v>43</v>
       </c>
@@ -5733,7 +5753,7 @@
       <c r="G161" s="1"/>
     </row>
     <row r="162" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A162" s="35" t="s">
+      <c r="A162" s="28" t="s">
         <v>312</v>
       </c>
       <c r="B162" s="1"/>
@@ -5745,12 +5765,12 @@
       <c r="F162" s="7">
         <v>13</v>
       </c>
-      <c r="G162" s="55" t="s">
-        <v>532</v>
+      <c r="G162" s="48" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A163" s="36"/>
+      <c r="A163" s="31"/>
       <c r="B163" s="1" t="s">
         <v>284</v>
       </c>
@@ -5763,7 +5783,7 @@
       <c r="G163" s="1"/>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A164" s="36"/>
+      <c r="A164" s="31"/>
       <c r="B164" s="1" t="s">
         <v>285</v>
       </c>
@@ -5776,7 +5796,7 @@
       <c r="G164" s="1"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A165" s="36"/>
+      <c r="A165" s="31"/>
       <c r="B165" s="1" t="s">
         <v>253</v>
       </c>
@@ -5789,7 +5809,7 @@
       <c r="G165" s="1"/>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A166" s="36"/>
+      <c r="A166" s="31"/>
       <c r="B166" s="1" t="s">
         <v>314</v>
       </c>
@@ -5802,7 +5822,7 @@
       <c r="G166" s="1"/>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A167" s="37"/>
+      <c r="A167" s="29"/>
       <c r="B167" s="1" t="s">
         <v>315</v>
       </c>
@@ -5815,7 +5835,7 @@
       <c r="G167" s="1"/>
     </row>
     <row r="168" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A168" s="35" t="s">
+      <c r="A168" s="28" t="s">
         <v>45</v>
       </c>
       <c r="B168" s="1"/>
@@ -5834,7 +5854,7 @@
       <c r="G168" s="1"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A169" s="37"/>
+      <c r="A169" s="29"/>
       <c r="B169" s="1" t="s">
         <v>346</v>
       </c>
@@ -5847,7 +5867,7 @@
       <c r="G169" s="1"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A170" s="44" t="s">
+      <c r="A170" s="33" t="s">
         <v>347</v>
       </c>
       <c r="B170" s="7" t="s">
@@ -5868,7 +5888,7 @@
       <c r="G170" s="1"/>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A171" s="45"/>
+      <c r="A171" s="25"/>
       <c r="B171" s="7" t="s">
         <v>47</v>
       </c>
@@ -5887,7 +5907,7 @@
       <c r="G171" s="1"/>
     </row>
     <row r="172" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A172" s="45"/>
+      <c r="A172" s="25"/>
       <c r="B172" s="7" t="s">
         <v>297</v>
       </c>
@@ -5906,7 +5926,7 @@
       <c r="G172" s="1"/>
     </row>
     <row r="173" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A173" s="41"/>
+      <c r="A173" s="26"/>
       <c r="B173" s="7" t="s">
         <v>49</v>
       </c>
@@ -5942,7 +5962,7 @@
       <c r="G174" s="1"/>
     </row>
     <row r="175" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A175" s="39" t="s">
+      <c r="A175" s="32" t="s">
         <v>6</v>
       </c>
       <c r="B175" s="3"/>
@@ -5957,7 +5977,7 @@
       <c r="G175" s="1"/>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A176" s="39"/>
+      <c r="A176" s="32"/>
       <c r="B176" s="3" t="s">
         <v>69</v>
       </c>
@@ -5970,7 +5990,7 @@
       <c r="G176" s="1"/>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A177" s="39"/>
+      <c r="A177" s="32"/>
       <c r="B177" s="3" t="s">
         <v>72</v>
       </c>
@@ -5983,7 +6003,7 @@
       <c r="G177" s="1"/>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A178" s="39"/>
+      <c r="A178" s="32"/>
       <c r="B178" s="3" t="s">
         <v>176</v>
       </c>
@@ -5996,7 +6016,7 @@
       <c r="G178" s="1"/>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A179" s="39"/>
+      <c r="A179" s="32"/>
       <c r="B179" s="3" t="s">
         <v>177</v>
       </c>
@@ -6009,7 +6029,7 @@
       <c r="G179" s="1"/>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A180" s="39"/>
+      <c r="A180" s="32"/>
       <c r="B180" s="3" t="s">
         <v>178</v>
       </c>
@@ -6022,7 +6042,7 @@
       <c r="G180" s="1"/>
     </row>
     <row r="181" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A181" s="35" t="s">
+      <c r="A181" s="28" t="s">
         <v>60</v>
       </c>
       <c r="B181" s="1"/>
@@ -6037,7 +6057,7 @@
       <c r="G181" s="1"/>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A182" s="36"/>
+      <c r="A182" s="31"/>
       <c r="B182" s="6" t="s">
         <v>60</v>
       </c>
@@ -6052,7 +6072,7 @@
       <c r="G182" s="1"/>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A183" s="36"/>
+      <c r="A183" s="31"/>
       <c r="B183" s="6" t="s">
         <v>319</v>
       </c>
@@ -6067,7 +6087,7 @@
       <c r="G183" s="1"/>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A184" s="36"/>
+      <c r="A184" s="31"/>
       <c r="B184" s="6" t="s">
         <v>285</v>
       </c>
@@ -6082,7 +6102,7 @@
       <c r="G184" s="1"/>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A185" s="36"/>
+      <c r="A185" s="31"/>
       <c r="B185" s="6" t="s">
         <v>322</v>
       </c>
@@ -6097,7 +6117,7 @@
       <c r="G185" s="1"/>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A186" s="36"/>
+      <c r="A186" s="31"/>
       <c r="B186" s="6" t="s">
         <v>324</v>
       </c>
@@ -6112,7 +6132,7 @@
       <c r="G186" s="1"/>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A187" s="36"/>
+      <c r="A187" s="31"/>
       <c r="B187" s="6" t="s">
         <v>326</v>
       </c>
@@ -6127,7 +6147,7 @@
       <c r="G187" s="1"/>
     </row>
     <row r="188" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A188" s="36"/>
+      <c r="A188" s="31"/>
       <c r="B188" s="6" t="s">
         <v>328</v>
       </c>
@@ -6142,7 +6162,7 @@
       <c r="G188" s="1"/>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A189" s="36"/>
+      <c r="A189" s="31"/>
       <c r="B189" s="6" t="s">
         <v>330</v>
       </c>
@@ -6157,7 +6177,7 @@
       <c r="G189" s="1"/>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A190" s="36"/>
+      <c r="A190" s="31"/>
       <c r="B190" s="6" t="s">
         <v>332</v>
       </c>
@@ -6172,7 +6192,7 @@
       <c r="G190" s="1"/>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A191" s="37"/>
+      <c r="A191" s="29"/>
       <c r="B191" s="6" t="s">
         <v>334</v>
       </c>
@@ -6187,7 +6207,7 @@
       <c r="G191" s="1"/>
     </row>
     <row r="192" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A192" s="35" t="s">
+      <c r="A192" s="28" t="s">
         <v>61</v>
       </c>
       <c r="B192" s="1"/>
@@ -6202,7 +6222,7 @@
       <c r="G192" s="1"/>
     </row>
     <row r="193" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A193" s="36"/>
+      <c r="A193" s="31"/>
       <c r="B193" s="6" t="s">
         <v>60</v>
       </c>
@@ -6217,7 +6237,7 @@
       <c r="G193" s="1"/>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A194" s="36"/>
+      <c r="A194" s="31"/>
       <c r="B194" s="6" t="s">
         <v>61</v>
       </c>
@@ -6232,7 +6252,7 @@
       <c r="G194" s="1"/>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A195" s="36"/>
+      <c r="A195" s="31"/>
       <c r="B195" s="6" t="s">
         <v>285</v>
       </c>
@@ -6247,7 +6267,7 @@
       <c r="G195" s="1"/>
     </row>
     <row r="196" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A196" s="36"/>
+      <c r="A196" s="31"/>
       <c r="B196" s="6" t="s">
         <v>328</v>
       </c>
@@ -6262,7 +6282,7 @@
       <c r="G196" s="1"/>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A197" s="36"/>
+      <c r="A197" s="31"/>
       <c r="B197" s="6" t="s">
         <v>341</v>
       </c>
@@ -6277,7 +6297,7 @@
       <c r="G197" s="1"/>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A198" s="36"/>
+      <c r="A198" s="31"/>
       <c r="B198" s="6" t="s">
         <v>343</v>
       </c>
@@ -6292,7 +6312,7 @@
       <c r="G198" s="1"/>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A199" s="36"/>
+      <c r="A199" s="31"/>
       <c r="B199" s="6" t="s">
         <v>348</v>
       </c>
@@ -6307,7 +6327,7 @@
       <c r="G199" s="1"/>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A200" s="36"/>
+      <c r="A200" s="31"/>
       <c r="B200" s="6" t="s">
         <v>350</v>
       </c>
@@ -6322,7 +6342,7 @@
       <c r="G200" s="1"/>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A201" s="36"/>
+      <c r="A201" s="31"/>
       <c r="B201" s="6" t="s">
         <v>352</v>
       </c>
@@ -6337,7 +6357,7 @@
       <c r="G201" s="1"/>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A202" s="37"/>
+      <c r="A202" s="29"/>
       <c r="B202" s="6" t="s">
         <v>111</v>
       </c>
@@ -6352,7 +6372,7 @@
       <c r="G202" s="1"/>
     </row>
     <row r="203" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A203" s="42" t="s">
+      <c r="A203" s="27" t="s">
         <v>62</v>
       </c>
       <c r="B203" s="1"/>
@@ -6367,7 +6387,7 @@
       <c r="G203" s="1"/>
     </row>
     <row r="204" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A204" s="42"/>
+      <c r="A204" s="27"/>
       <c r="B204" s="6" t="s">
         <v>60</v>
       </c>
@@ -6382,7 +6402,7 @@
       <c r="G204" s="1"/>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A205" s="42"/>
+      <c r="A205" s="27"/>
       <c r="B205" s="6" t="s">
         <v>61</v>
       </c>
@@ -6397,7 +6417,7 @@
       <c r="G205" s="1"/>
     </row>
     <row r="206" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A206" s="42"/>
+      <c r="A206" s="27"/>
       <c r="B206" s="6" t="s">
         <v>359</v>
       </c>
@@ -6412,7 +6432,7 @@
       <c r="G206" s="1"/>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A207" s="42"/>
+      <c r="A207" s="27"/>
       <c r="B207" s="6" t="s">
         <v>361</v>
       </c>
@@ -6427,7 +6447,7 @@
       <c r="G207" s="1"/>
     </row>
     <row r="208" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A208" s="42"/>
+      <c r="A208" s="27"/>
       <c r="B208" s="6" t="s">
         <v>363</v>
       </c>
@@ -6442,7 +6462,7 @@
       <c r="G208" s="1"/>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A209" s="42"/>
+      <c r="A209" s="27"/>
       <c r="B209" s="6" t="s">
         <v>365</v>
       </c>
@@ -6457,7 +6477,7 @@
       <c r="G209" s="1"/>
     </row>
     <row r="210" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A210" s="42"/>
+      <c r="A210" s="27"/>
       <c r="B210" s="6" t="s">
         <v>367</v>
       </c>
@@ -6472,7 +6492,7 @@
       <c r="G210" s="1"/>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A211" s="42"/>
+      <c r="A211" s="27"/>
       <c r="B211" s="6" t="s">
         <v>369</v>
       </c>
@@ -6487,7 +6507,7 @@
       <c r="G211" s="1"/>
     </row>
     <row r="212" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A212" s="42"/>
+      <c r="A212" s="27"/>
       <c r="B212" s="6" t="s">
         <v>371</v>
       </c>
@@ -6502,7 +6522,7 @@
       <c r="G212" s="1"/>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A213" s="42"/>
+      <c r="A213" s="27"/>
       <c r="B213" s="6" t="s">
         <v>373</v>
       </c>
@@ -6517,7 +6537,7 @@
       <c r="G213" s="1"/>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A214" s="42"/>
+      <c r="A214" s="27"/>
       <c r="B214" s="6" t="s">
         <v>375</v>
       </c>
@@ -6532,7 +6552,7 @@
       <c r="G214" s="1"/>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A215" s="42"/>
+      <c r="A215" s="27"/>
       <c r="B215" s="6" t="s">
         <v>377</v>
       </c>
@@ -6547,7 +6567,7 @@
       <c r="G215" s="1"/>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A216" s="42"/>
+      <c r="A216" s="27"/>
       <c r="B216" s="6" t="s">
         <v>379</v>
       </c>
@@ -6562,7 +6582,7 @@
       <c r="G216" s="1"/>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A217" s="42"/>
+      <c r="A217" s="27"/>
       <c r="B217" s="6" t="s">
         <v>381</v>
       </c>
@@ -6577,7 +6597,7 @@
       <c r="G217" s="1"/>
     </row>
     <row r="218" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A218" s="42"/>
+      <c r="A218" s="27"/>
       <c r="B218" s="6" t="s">
         <v>383</v>
       </c>
@@ -6592,7 +6612,7 @@
       <c r="G218" s="1"/>
     </row>
     <row r="219" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A219" s="42"/>
+      <c r="A219" s="27"/>
       <c r="B219" s="6" t="s">
         <v>385</v>
       </c>
@@ -6607,7 +6627,7 @@
       <c r="G219" s="1"/>
     </row>
     <row r="220" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A220" s="42"/>
+      <c r="A220" s="27"/>
       <c r="B220" s="6" t="s">
         <v>387</v>
       </c>
@@ -6622,7 +6642,7 @@
       <c r="G220" s="1"/>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A221" s="42"/>
+      <c r="A221" s="27"/>
       <c r="B221" s="6" t="s">
         <v>389</v>
       </c>
@@ -6637,7 +6657,7 @@
       <c r="G221" s="1"/>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A222" s="42"/>
+      <c r="A222" s="27"/>
       <c r="B222" s="6" t="s">
         <v>111</v>
       </c>
@@ -6652,7 +6672,7 @@
       <c r="G222" s="1"/>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A223" s="42"/>
+      <c r="A223" s="27"/>
       <c r="B223" s="6" t="s">
         <v>392</v>
       </c>
@@ -6667,7 +6687,7 @@
       <c r="G223" s="1"/>
     </row>
     <row r="224" spans="1:7" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A224" s="42" t="s">
+      <c r="A224" s="27" t="s">
         <v>63</v>
       </c>
       <c r="B224" s="1"/>
@@ -6682,7 +6702,7 @@
       <c r="G224" s="1"/>
     </row>
     <row r="225" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A225" s="42"/>
+      <c r="A225" s="27"/>
       <c r="B225" s="6" t="s">
         <v>60</v>
       </c>
@@ -6697,7 +6717,7 @@
       <c r="G225" s="1"/>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A226" s="42"/>
+      <c r="A226" s="27"/>
       <c r="B226" s="6" t="s">
         <v>61</v>
       </c>
@@ -6712,7 +6732,7 @@
       <c r="G226" s="1"/>
     </row>
     <row r="227" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A227" s="42"/>
+      <c r="A227" s="27"/>
       <c r="B227" s="6" t="s">
         <v>359</v>
       </c>
@@ -6727,7 +6747,7 @@
       <c r="G227" s="1"/>
     </row>
     <row r="228" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A228" s="42"/>
+      <c r="A228" s="27"/>
       <c r="B228" s="6" t="s">
         <v>361</v>
       </c>
@@ -6742,7 +6762,7 @@
       <c r="G228" s="1"/>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A229" s="42"/>
+      <c r="A229" s="27"/>
       <c r="B229" s="6" t="s">
         <v>398</v>
       </c>
@@ -6757,7 +6777,7 @@
       <c r="G229" s="1"/>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A230" s="42"/>
+      <c r="A230" s="27"/>
       <c r="B230" s="6" t="s">
         <v>400</v>
       </c>
@@ -6772,7 +6792,7 @@
       <c r="G230" s="1"/>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A231" s="42"/>
+      <c r="A231" s="27"/>
       <c r="B231" s="6" t="s">
         <v>402</v>
       </c>
@@ -6787,7 +6807,7 @@
       <c r="G231" s="1"/>
     </row>
     <row r="232" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A232" s="42"/>
+      <c r="A232" s="27"/>
       <c r="B232" s="6" t="s">
         <v>365</v>
       </c>
@@ -6802,7 +6822,7 @@
       <c r="G232" s="1"/>
     </row>
     <row r="233" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A233" s="42"/>
+      <c r="A233" s="27"/>
       <c r="B233" s="6" t="s">
         <v>367</v>
       </c>
@@ -6817,7 +6837,7 @@
       <c r="G233" s="1"/>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A234" s="42"/>
+      <c r="A234" s="27"/>
       <c r="B234" s="6" t="s">
         <v>406</v>
       </c>
@@ -6832,7 +6852,7 @@
       <c r="G234" s="1"/>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A235" s="42"/>
+      <c r="A235" s="27"/>
       <c r="B235" s="6" t="s">
         <v>373</v>
       </c>
@@ -6847,7 +6867,7 @@
       <c r="G235" s="1"/>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A236" s="42"/>
+      <c r="A236" s="27"/>
       <c r="B236" s="6" t="s">
         <v>375</v>
       </c>
@@ -6862,7 +6882,7 @@
       <c r="G236" s="1"/>
     </row>
     <row r="237" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A237" s="42"/>
+      <c r="A237" s="27"/>
       <c r="B237" s="6" t="s">
         <v>410</v>
       </c>
@@ -6877,7 +6897,7 @@
       <c r="G237" s="1"/>
     </row>
     <row r="238" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A238" s="42"/>
+      <c r="A238" s="27"/>
       <c r="B238" s="6" t="s">
         <v>412</v>
       </c>
@@ -6892,7 +6912,7 @@
       <c r="G238" s="1"/>
     </row>
     <row r="239" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A239" s="42"/>
+      <c r="A239" s="27"/>
       <c r="B239" s="6" t="s">
         <v>414</v>
       </c>
@@ -6907,7 +6927,7 @@
       <c r="G239" s="1"/>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A240" s="42"/>
+      <c r="A240" s="27"/>
       <c r="B240" s="6" t="s">
         <v>389</v>
       </c>
@@ -6922,7 +6942,7 @@
       <c r="G240" s="1"/>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A241" s="42"/>
+      <c r="A241" s="27"/>
       <c r="B241" s="6" t="s">
         <v>111</v>
       </c>
@@ -6937,7 +6957,7 @@
       <c r="G241" s="1"/>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A242" s="42"/>
+      <c r="A242" s="27"/>
       <c r="B242" s="6" t="s">
         <v>392</v>
       </c>
@@ -6952,7 +6972,7 @@
       <c r="G242" s="1"/>
     </row>
     <row r="243" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A243" s="43" t="s">
+      <c r="A243" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B243" s="1"/>
@@ -6967,7 +6987,7 @@
       <c r="G243" s="1"/>
     </row>
     <row r="244" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A244" s="43"/>
+      <c r="A244" s="30"/>
       <c r="B244" s="6" t="s">
         <v>60</v>
       </c>
@@ -6982,7 +7002,7 @@
       <c r="G244" s="1"/>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A245" s="43"/>
+      <c r="A245" s="30"/>
       <c r="B245" s="6" t="s">
         <v>61</v>
       </c>
@@ -6997,7 +7017,7 @@
       <c r="G245" s="1"/>
     </row>
     <row r="246" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A246" s="43"/>
+      <c r="A246" s="30"/>
       <c r="B246" s="6" t="s">
         <v>359</v>
       </c>
@@ -7012,7 +7032,7 @@
       <c r="G246" s="1"/>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A247" s="43"/>
+      <c r="A247" s="30"/>
       <c r="B247" s="6" t="s">
         <v>361</v>
       </c>
@@ -7027,7 +7047,7 @@
       <c r="G247" s="1"/>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A248" s="43"/>
+      <c r="A248" s="30"/>
       <c r="B248" s="6" t="s">
         <v>398</v>
       </c>
@@ -7042,7 +7062,7 @@
       <c r="G248" s="1"/>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A249" s="43"/>
+      <c r="A249" s="30"/>
       <c r="B249" s="6" t="s">
         <v>425</v>
       </c>
@@ -7057,7 +7077,7 @@
       <c r="G249" s="1"/>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A250" s="43"/>
+      <c r="A250" s="30"/>
       <c r="B250" s="6" t="s">
         <v>427</v>
       </c>
@@ -7072,7 +7092,7 @@
       <c r="G250" s="1"/>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A251" s="43"/>
+      <c r="A251" s="30"/>
       <c r="B251" s="6" t="s">
         <v>365</v>
       </c>
@@ -7087,7 +7107,7 @@
       <c r="G251" s="1"/>
     </row>
     <row r="252" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A252" s="43"/>
+      <c r="A252" s="30"/>
       <c r="B252" s="6" t="s">
         <v>430</v>
       </c>
@@ -7102,7 +7122,7 @@
       <c r="G252" s="1"/>
     </row>
     <row r="253" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A253" s="43"/>
+      <c r="A253" s="30"/>
       <c r="B253" s="6" t="s">
         <v>432</v>
       </c>
@@ -7117,7 +7137,7 @@
       <c r="G253" s="1"/>
     </row>
     <row r="254" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A254" s="42" t="s">
+      <c r="A254" s="27" t="s">
         <v>65</v>
       </c>
       <c r="B254" s="1"/>
@@ -7132,7 +7152,7 @@
       <c r="G254" s="1"/>
     </row>
     <row r="255" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A255" s="42"/>
+      <c r="A255" s="27"/>
       <c r="B255" s="6" t="s">
         <v>60</v>
       </c>
@@ -7147,7 +7167,7 @@
       <c r="G255" s="1"/>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A256" s="42"/>
+      <c r="A256" s="27"/>
       <c r="B256" s="6" t="s">
         <v>61</v>
       </c>
@@ -7162,7 +7182,7 @@
       <c r="G256" s="1"/>
     </row>
     <row r="257" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A257" s="42"/>
+      <c r="A257" s="27"/>
       <c r="B257" s="6" t="s">
         <v>359</v>
       </c>
@@ -7177,7 +7197,7 @@
       <c r="G257" s="1"/>
     </row>
     <row r="258" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A258" s="42"/>
+      <c r="A258" s="27"/>
       <c r="B258" s="6" t="s">
         <v>361</v>
       </c>
@@ -7192,7 +7212,7 @@
       <c r="G258" s="1"/>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A259" s="42"/>
+      <c r="A259" s="27"/>
       <c r="B259" s="6" t="s">
         <v>398</v>
       </c>
@@ -7207,7 +7227,7 @@
       <c r="G259" s="1"/>
     </row>
     <row r="260" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A260" s="42"/>
+      <c r="A260" s="27"/>
       <c r="B260" s="6" t="s">
         <v>440</v>
       </c>
@@ -7222,7 +7242,7 @@
       <c r="G260" s="1"/>
     </row>
     <row r="261" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A261" s="42"/>
+      <c r="A261" s="27"/>
       <c r="B261" s="6" t="s">
         <v>442</v>
       </c>
@@ -7237,7 +7257,7 @@
       <c r="G261" s="1"/>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A262" s="42"/>
+      <c r="A262" s="27"/>
       <c r="B262" s="6" t="s">
         <v>365</v>
       </c>
@@ -7252,7 +7272,7 @@
       <c r="G262" s="1"/>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A263" s="42"/>
+      <c r="A263" s="27"/>
       <c r="B263" s="6" t="s">
         <v>367</v>
       </c>
@@ -7267,7 +7287,7 @@
       <c r="G263" s="1"/>
     </row>
     <row r="264" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A264" s="42"/>
+      <c r="A264" s="27"/>
       <c r="B264" s="6" t="s">
         <v>373</v>
       </c>
@@ -7282,7 +7302,7 @@
       <c r="G264" s="1"/>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A265" s="42"/>
+      <c r="A265" s="27"/>
       <c r="B265" s="6" t="s">
         <v>447</v>
       </c>
@@ -7297,7 +7317,7 @@
       <c r="G265" s="1"/>
     </row>
     <row r="266" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A266" s="42"/>
+      <c r="A266" s="27"/>
       <c r="B266" s="6" t="s">
         <v>449</v>
       </c>
@@ -7312,7 +7332,7 @@
       <c r="G266" s="1"/>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A267" s="42"/>
+      <c r="A267" s="27"/>
       <c r="B267" s="6" t="s">
         <v>451</v>
       </c>
@@ -7327,7 +7347,7 @@
       <c r="G267" s="1"/>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A268" s="42"/>
+      <c r="A268" s="27"/>
       <c r="B268" s="6" t="s">
         <v>453</v>
       </c>
@@ -7342,7 +7362,7 @@
       <c r="G268" s="1"/>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A269" s="42"/>
+      <c r="A269" s="27"/>
       <c r="B269" s="6" t="s">
         <v>389</v>
       </c>
@@ -7357,7 +7377,7 @@
       <c r="G269" s="1"/>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A270" s="42"/>
+      <c r="A270" s="27"/>
       <c r="B270" s="6" t="s">
         <v>455</v>
       </c>
@@ -7372,7 +7392,7 @@
       <c r="G270" s="1"/>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A271" s="42"/>
+      <c r="A271" s="27"/>
       <c r="B271" s="6" t="s">
         <v>111</v>
       </c>
@@ -7387,7 +7407,7 @@
       <c r="G271" s="1"/>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A272" s="42"/>
+      <c r="A272" s="27"/>
       <c r="B272" s="6" t="s">
         <v>392</v>
       </c>
@@ -7402,7 +7422,7 @@
       <c r="G272" s="1"/>
     </row>
     <row r="273" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A273" s="42" t="s">
+      <c r="A273" s="27" t="s">
         <v>66</v>
       </c>
       <c r="B273" s="1"/>
@@ -7417,7 +7437,7 @@
       <c r="G273" s="1"/>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A274" s="42"/>
+      <c r="A274" s="27"/>
       <c r="B274" s="6" t="s">
         <v>60</v>
       </c>
@@ -7432,7 +7452,7 @@
       <c r="G274" s="1"/>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A275" s="42"/>
+      <c r="A275" s="27"/>
       <c r="B275" s="6" t="s">
         <v>61</v>
       </c>
@@ -7447,7 +7467,7 @@
       <c r="G275" s="1"/>
     </row>
     <row r="276" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A276" s="42"/>
+      <c r="A276" s="27"/>
       <c r="B276" s="6" t="s">
         <v>359</v>
       </c>
@@ -7462,7 +7482,7 @@
       <c r="G276" s="1"/>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A277" s="42"/>
+      <c r="A277" s="27"/>
       <c r="B277" s="6" t="s">
         <v>410</v>
       </c>
@@ -7477,7 +7497,7 @@
       <c r="G277" s="1"/>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A278" s="42"/>
+      <c r="A278" s="27"/>
       <c r="B278" s="6" t="s">
         <v>464</v>
       </c>
@@ -7492,7 +7512,7 @@
       <c r="G278" s="1"/>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A279" s="42"/>
+      <c r="A279" s="27"/>
       <c r="B279" s="6" t="s">
         <v>466</v>
       </c>
@@ -7507,7 +7527,7 @@
       <c r="G279" s="1"/>
     </row>
     <row r="280" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A280" s="42"/>
+      <c r="A280" s="27"/>
       <c r="B280" s="6" t="s">
         <v>365</v>
       </c>
@@ -7522,7 +7542,7 @@
       <c r="G280" s="1"/>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A281" s="42"/>
+      <c r="A281" s="27"/>
       <c r="B281" s="6" t="s">
         <v>367</v>
       </c>
@@ -7537,7 +7557,7 @@
       <c r="G281" s="1"/>
     </row>
     <row r="282" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A282" s="42"/>
+      <c r="A282" s="27"/>
       <c r="B282" s="6" t="s">
         <v>373</v>
       </c>
@@ -7552,7 +7572,7 @@
       <c r="G282" s="1"/>
     </row>
     <row r="283" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A283" s="42"/>
+      <c r="A283" s="27"/>
       <c r="B283" s="6" t="s">
         <v>471</v>
       </c>
@@ -7567,7 +7587,7 @@
       <c r="G283" s="1"/>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A284" s="42"/>
+      <c r="A284" s="27"/>
       <c r="B284" s="6" t="s">
         <v>473</v>
       </c>
@@ -7582,7 +7602,7 @@
       <c r="G284" s="1"/>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A285" s="42"/>
+      <c r="A285" s="27"/>
       <c r="B285" s="6" t="s">
         <v>475</v>
       </c>
@@ -7597,7 +7617,7 @@
       <c r="G285" s="1"/>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A286" s="42"/>
+      <c r="A286" s="27"/>
       <c r="B286" s="6" t="s">
         <v>477</v>
       </c>
@@ -7612,7 +7632,7 @@
       <c r="G286" s="1"/>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A287" s="42"/>
+      <c r="A287" s="27"/>
       <c r="B287" s="6" t="s">
         <v>479</v>
       </c>
@@ -7627,7 +7647,7 @@
       <c r="G287" s="1"/>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A288" s="42"/>
+      <c r="A288" s="27"/>
       <c r="B288" s="6" t="s">
         <v>481</v>
       </c>
@@ -7642,83 +7662,69 @@
       <c r="G288" s="1"/>
     </row>
     <row r="289" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A289" s="52" t="s">
+      <c r="A289" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="B289" s="53"/>
-      <c r="C289" s="54" t="s">
+      <c r="B289" s="54"/>
+      <c r="C289" s="55" t="s">
         <v>306</v>
       </c>
-      <c r="D289" s="53"/>
+      <c r="D289" s="54"/>
       <c r="E289" s="56" t="s">
-        <v>535</v>
-      </c>
-      <c r="F289" s="53">
+        <v>533</v>
+      </c>
+      <c r="F289" s="54">
         <v>11</v>
       </c>
       <c r="G289" s="1"/>
     </row>
-    <row r="290" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A290" s="52" t="s">
+    <row r="290" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A290" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="B290" s="53"/>
-      <c r="C290" s="54" t="s">
+      <c r="B290" s="54"/>
+      <c r="C290" s="55" t="s">
         <v>307</v>
       </c>
-      <c r="D290" s="53"/>
-      <c r="E290" s="45"/>
-      <c r="F290" s="53">
+      <c r="D290" s="54"/>
+      <c r="E290" s="57"/>
+      <c r="F290" s="54">
         <v>11</v>
       </c>
       <c r="G290" s="1"/>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A291" s="52"/>
-      <c r="B291" s="53" t="s">
+      <c r="A291" s="53"/>
+      <c r="B291" s="54" t="s">
         <v>308</v>
       </c>
-      <c r="C291" s="54" t="s">
+      <c r="C291" s="55" t="s">
         <v>309</v>
       </c>
-      <c r="D291" s="53"/>
-      <c r="E291" s="45"/>
-      <c r="F291" s="53">
+      <c r="D291" s="54"/>
+      <c r="E291" s="57"/>
+      <c r="F291" s="54">
         <v>11</v>
       </c>
       <c r="G291" s="1"/>
     </row>
     <row r="292" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A292" s="52" t="s">
+      <c r="A292" s="53" t="s">
         <v>310</v>
       </c>
-      <c r="B292" s="53"/>
-      <c r="C292" s="54" t="s">
+      <c r="B292" s="54"/>
+      <c r="C292" s="55" t="s">
         <v>311</v>
       </c>
-      <c r="D292" s="53"/>
-      <c r="E292" s="41"/>
-      <c r="F292" s="53">
+      <c r="D292" s="54"/>
+      <c r="E292" s="58"/>
+      <c r="F292" s="54">
         <v>11</v>
       </c>
       <c r="G292" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E289:E292"/>
-    <mergeCell ref="A254:A272"/>
-    <mergeCell ref="A273:A288"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A203:A223"/>
-    <mergeCell ref="A224:A242"/>
-    <mergeCell ref="A243:A253"/>
-    <mergeCell ref="A181:A191"/>
-    <mergeCell ref="A192:A202"/>
-    <mergeCell ref="A175:A180"/>
-    <mergeCell ref="A168:A169"/>
-    <mergeCell ref="A170:A173"/>
-    <mergeCell ref="A162:A167"/>
     <mergeCell ref="A2:A28"/>
     <mergeCell ref="A29:A54"/>
     <mergeCell ref="A55:A60"/>
@@ -7735,6 +7741,20 @@
     <mergeCell ref="A105:A107"/>
     <mergeCell ref="A108:A109"/>
     <mergeCell ref="A110:A115"/>
+    <mergeCell ref="E289:E292"/>
+    <mergeCell ref="A254:A272"/>
+    <mergeCell ref="A273:A288"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A203:A223"/>
+    <mergeCell ref="A224:A242"/>
+    <mergeCell ref="A243:A253"/>
+    <mergeCell ref="A181:A191"/>
+    <mergeCell ref="A192:A202"/>
+    <mergeCell ref="A175:A180"/>
+    <mergeCell ref="A168:A169"/>
+    <mergeCell ref="A170:A173"/>
+    <mergeCell ref="A162:A167"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1"/>

</xml_diff>